<commit_message>
Change the loans in Specified Non Competitive rates [ref #3]
</commit_message>
<xml_diff>
--- a/doc/InOutEngine/6_with_out_exceptions.xlsx
+++ b/doc/InOutEngine/6_with_out_exceptions.xlsx
@@ -14,6 +14,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
     <definedName function="false" hidden="false" name="_xlnm._FilterDatabase" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
+    <definedName function="false" hidden="false" name="_xlnm._FilterDatabase_1" vbProcedure="false">'bid input'!$A$1:$N$21</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -684,20 +685,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="13">
+  <numFmts count="12">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="H:MM:SS\ AM/PM;@" numFmtId="165"/>
     <numFmt formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)" numFmtId="166"/>
     <numFmt formatCode="0%" numFmtId="167"/>
     <numFmt formatCode="0.000%" numFmtId="168"/>
     <numFmt formatCode="M/D/YY\ H:MM\ AM/PM;@" numFmtId="169"/>
-    <numFmt formatCode="GENERAL" numFmtId="170"/>
-    <numFmt formatCode="M/D/YYYY\ H:MM" numFmtId="171"/>
-    <numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)" numFmtId="172"/>
-    <numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)" numFmtId="173"/>
-    <numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* \-??_);_(@_)" numFmtId="174"/>
-    <numFmt formatCode="0.00%" numFmtId="175"/>
-    <numFmt formatCode="0.0%" numFmtId="176"/>
+    <numFmt formatCode="M/D/YYYY\ H:MM" numFmtId="170"/>
+    <numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)" numFmtId="171"/>
+    <numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)" numFmtId="172"/>
+    <numFmt formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* \-??_);_(@_)" numFmtId="173"/>
+    <numFmt formatCode="0.00%" numFmtId="174"/>
+    <numFmt formatCode="0.0%" numFmtId="175"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -910,7 +910,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="172">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="171">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -925,7 +925,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -949,9 +949,9 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="169" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="171" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
@@ -1008,18 +1008,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="173" xfId="15">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="15">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="173" xfId="15">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="172" xfId="15">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1031,7 +1028,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="172" xfId="15">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="171" xfId="15">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1043,13 +1040,13 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="174" xfId="15">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="173" xfId="15">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="173" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="175" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="174" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="17">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -1065,11 +1062,11 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="168" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="168" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="175" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="174" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="168" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="176" xfId="19">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="175" xfId="19">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1164,21 +1161,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3450980392157"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4901960784314"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.9176470588235"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3372549019608"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.75294117647059"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0745098039216"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.46666666666667"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.8980392156863"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5529411764706"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.9843137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3882352941176"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.79607843137255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9960784313726"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="9.50196078431373"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="10.9411764705882"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="12.0980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.92941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="1" s="2">
@@ -2386,29 +2383,29 @@
   </sheetPr>
   <dimension ref="A1:U220"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="G64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="K149" activeCellId="0" pane="topLeft" sqref="K149"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="E22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F34" activeCellId="0" pane="topLeft" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9137254901961"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.0588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.2196078431373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9137254901961"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9098039215686"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.17647058823529"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.4980392156863"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9176470588235"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.89019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.956862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.5372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.2980392156863"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.9803921568627"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.9686274509804"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.21176470588235"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.5686274509804"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9843137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.92941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -3733,23 +3730,26 @@
       <c r="F36" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="29" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="H36" s="29" t="inlineStr">
-        <f aca="false">+G36</f>
+      <c r="G36" s="29" t="inlineStr">
+        <f aca="false">F23</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I36" s="29" t="inlineStr">
-        <f aca="false">+H36</f>
+      <c r="H36" s="29" t="inlineStr">
+        <f aca="false">F11</f>
         <is>
           <t/>
         </is>
       </c>
+      <c r="I36" s="29" t="inlineStr">
+        <f aca="false">F15</f>
+        <is>
+          <t/>
+        </is>
+      </c>
       <c r="J36" s="29" t="inlineStr">
-        <f aca="false">+I36</f>
+        <f aca="false">I36</f>
         <is>
           <t/>
         </is>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="M59" s="27" t="n">
         <f aca="false">+IF(M58=0,0,SUMPRODUCT(G58:L58,G59:L59)/M58)</f>
-        <v>0.035</v>
+        <v>0.0275223370366271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="60">
@@ -4959,15 +4959,15 @@
       <c r="F67" s="40"/>
       <c r="G67" s="41" t="n">
         <f aca="false">+IF(ISERR(IF(ISERR((G29*G30)+(G58*G59))/(G58+G29),G59,((G29*G30)+(G58*G59))/(G58+G29))),0,IF(ISERR((G29*G30)+(G58*G59))/(G58+G29),G59,((G29*G30)+(G58*G59))/(G58+G29)))</f>
-        <v>0.028625</v>
+        <v>0.024625</v>
       </c>
       <c r="H67" s="41" t="n">
         <f aca="false">+IF(ISERR(IF(ISERR((H29*H30)+(H58*H59))/(H58+H29),H59,((H29*H30)+(H58*H59))/(H58+H29))),0,IF(ISERR((H29*H30)+(H58*H59))/(H58+H29),H59,((H29*H30)+(H58*H59))/(H58+H29)))</f>
-        <v>0.0297916666666667</v>
+        <v>0.0239583333333333</v>
       </c>
       <c r="I67" s="41" t="n">
         <f aca="false">+IF(ISERR(IF(ISERR((I29*I30)+(I58*I59))/(I58+I29),I59,((I29*I30)+(I58*I59))/(I58+I29))),0,IF(ISERR((I29*I30)+(I58*I59))/(I58+I29),I59,((I29*I30)+(I58*I59))/(I58+I29)))</f>
-        <v>0.03125</v>
+        <v>0.0275</v>
       </c>
       <c r="J67" s="41" t="inlineStr">
         <f aca="false">+IF(ISERR(IF(ISERR((J29*J30)+(J58*J59))/(J58+J29),J59,((J29*J30)+(J58*J59))/(J58+J29))),0,IF(ISERR((J29*J30)+(J58*J59))/(J58+J29),J59,((J29*J30)+(J58*J59))/(J58+J29)))</f>
@@ -4989,7 +4989,7 @@
       </c>
       <c r="M67" s="42" t="n">
         <f aca="false">+IF(ISERR(IF(ISERR((M29*M30)+(M58*M59))/(M58+M29),M59,((M29*M30)+(M58*M59))/(M58+M29))),0,IF(ISERR((M29*M30)+(M58*M59))/(M58+M29),M59,((M29*M30)+(M58*M59))/(M58+M29)))</f>
-        <v>0.0314964217566043</v>
+        <v>0.0264397098340779</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="69">
@@ -5010,45 +5010,45 @@
       <c r="E70" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="F70" s="43"/>
-      <c r="G70" s="44" t="s">
+      <c r="F70" s="15"/>
+      <c r="G70" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="I70" s="43" t="s">
+      <c r="I70" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="J70" s="44" t="s">
+      <c r="J70" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="K70" s="44" t="s">
+      <c r="K70" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="L70" s="44" t="s">
+      <c r="L70" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="M70" s="44" t="s">
+      <c r="M70" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="N70" s="44" t="s">
+      <c r="N70" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="O70" s="44" t="s">
+      <c r="O70" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="P70" s="44" t="s">
+      <c r="P70" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="Q70" s="45"/>
-      <c r="R70" s="44" t="s">
+      <c r="Q70" s="44"/>
+      <c r="R70" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="S70" s="44" t="s">
+      <c r="S70" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="T70" s="44" t="s">
+      <c r="T70" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="U70" s="44" t="s">
+      <c r="U70" s="43" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5069,53 +5069,53 @@
         <f aca="false">+MIN('bid input'!D2,'bid input'!M2)</f>
         <v>187500</v>
       </c>
-      <c r="F71" s="46" t="n">
+      <c r="F71" s="45" t="n">
         <f aca="false">+IF(D71&gt;0,E71,0)</f>
         <v>0</v>
       </c>
-      <c r="G71" s="47" t="n">
+      <c r="G71" s="46" t="n">
         <f aca="false">+IF($F71&gt;0,RANK($D71,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H71" s="48" t="n">
+      <c r="H71" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B71,$J$96:$K$115,2,0)),0,VLOOKUP(B71,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I71" s="48" t="n">
+      <c r="I71" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B71,$J$96:$K$115,2,0)),0,VLOOKUP(B71,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J71" s="49" t="n">
+      <c r="J71" s="48" t="n">
         <f aca="false">VLOOKUP(B71,'bid input'!B:S,18,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="K71" s="47" t="str">
+      <c r="K71" s="46" t="str">
         <f aca="false">IF(G71=0,"",G71)</f>
         <v/>
       </c>
-      <c r="L71" s="47" t="n">
+      <c r="L71" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K71,K$71:K$90,1)),0,RANK(K71,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M71" s="50" t="n">
+      <c r="M71" s="49" t="n">
         <f aca="false">VALUE(L71&amp;J71)</f>
         <v>40928.625</v>
       </c>
-      <c r="N71" s="47" t="n">
+      <c r="N71" s="46" t="n">
         <f aca="false">IF(L71=0,0,COUNT(M$71:M$90)-(RANK(M71,M$71:M$90,0)+COUNTIF(M71:M$71,M71))+2)</f>
         <v>0</v>
       </c>
-      <c r="O71" s="51" t="inlineStr">
+      <c r="O71" s="50" t="inlineStr">
         <f aca="false">D71</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P71" s="52" t="n">
+      <c r="P71" s="51" t="n">
         <f aca="false">B71</f>
         <v>1104134</v>
       </c>
-      <c r="Q71" s="53"/>
+      <c r="Q71" s="52"/>
       <c r="R71" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5124,7 +5124,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T71" s="51" t="n">
+      <c r="T71" s="50" t="n">
         <f aca="false">VLOOKUP(S71,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5150,53 +5150,53 @@
         <f aca="false">+MIN('bid input'!D3,'bid input'!M3)</f>
         <v>500000</v>
       </c>
-      <c r="F72" s="46" t="n">
+      <c r="F72" s="45" t="n">
         <f aca="false">+IF(D72&gt;0,E72,0)</f>
         <v>0</v>
       </c>
-      <c r="G72" s="47" t="n">
+      <c r="G72" s="46" t="n">
         <f aca="false">+IF($F72&gt;0,RANK($D72,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H72" s="48" t="n">
+      <c r="H72" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B72,$J$96:$K$115,2,0)),0,VLOOKUP(B72,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I72" s="48" t="n">
+      <c r="I72" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B72,$J$96:$K$115,2,0)),0,VLOOKUP(B72,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J72" s="49" t="n">
+      <c r="J72" s="48" t="n">
         <f aca="false">VLOOKUP(B72,'bid input'!B:S,18,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="K72" s="47" t="str">
+      <c r="K72" s="46" t="str">
         <f aca="false">IF(G72=0,"",G72)</f>
         <v/>
       </c>
-      <c r="L72" s="47" t="n">
+      <c r="L72" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K72,K$71:K$90,1)),0,RANK(K72,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M72" s="50" t="n">
+      <c r="M72" s="49" t="n">
         <f aca="false">VALUE(L72&amp;J72)</f>
         <v>40928.625</v>
       </c>
-      <c r="N72" s="47" t="n">
+      <c r="N72" s="46" t="n">
         <f aca="false">IF(L72=0,0,COUNT(M$71:M$90)-(RANK(M72,M$71:M$90,0)+COUNTIF(M$71:M72,M72))+2)</f>
         <v>0</v>
       </c>
-      <c r="O72" s="51" t="inlineStr">
+      <c r="O72" s="50" t="inlineStr">
         <f aca="false">D72</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P72" s="52" t="n">
+      <c r="P72" s="51" t="n">
         <f aca="false">B72</f>
         <v>1104143</v>
       </c>
-      <c r="Q72" s="53"/>
+      <c r="Q72" s="52"/>
       <c r="R72" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5205,7 +5205,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T72" s="51" t="n">
+      <c r="T72" s="50" t="n">
         <f aca="false">VLOOKUP(S72,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5231,53 +5231,53 @@
         <f aca="false">+MIN('bid input'!D4,'bid input'!M4)</f>
         <v>185000</v>
       </c>
-      <c r="F73" s="46" t="n">
+      <c r="F73" s="45" t="n">
         <f aca="false">+IF(D73&gt;0,E73,0)</f>
         <v>0</v>
       </c>
-      <c r="G73" s="47" t="n">
+      <c r="G73" s="46" t="n">
         <f aca="false">+IF($F73&gt;0,RANK($D73,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H73" s="48" t="n">
+      <c r="H73" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B73,$J$96:$K$115,2,0)),0,VLOOKUP(B73,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I73" s="48" t="n">
+      <c r="I73" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B73,$J$96:$K$115,2,0)),0,VLOOKUP(B73,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J73" s="49" t="n">
+      <c r="J73" s="48" t="n">
         <f aca="false">VLOOKUP(B73,'bid input'!B:S,18,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="K73" s="47" t="str">
+      <c r="K73" s="46" t="str">
         <f aca="false">IF(G73=0,"",G73)</f>
         <v/>
       </c>
-      <c r="L73" s="47" t="n">
+      <c r="L73" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K73,K$71:K$90,1)),0,RANK(K73,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M73" s="50" t="n">
+      <c r="M73" s="49" t="n">
         <f aca="false">VALUE(L73&amp;J73)</f>
         <v>40928.625</v>
       </c>
-      <c r="N73" s="47" t="n">
+      <c r="N73" s="46" t="n">
         <f aca="false">IF(L73=0,0,COUNT(M$71:M$90)-(RANK(M73,M$71:M$90,0)+COUNTIF(M$71:M73,M73))+2)</f>
         <v>0</v>
       </c>
-      <c r="O73" s="51" t="inlineStr">
+      <c r="O73" s="50" t="inlineStr">
         <f aca="false">D73</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P73" s="52" t="n">
+      <c r="P73" s="51" t="n">
         <f aca="false">B73</f>
         <v>1104154</v>
       </c>
-      <c r="Q73" s="53"/>
+      <c r="Q73" s="52"/>
       <c r="R73" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5286,7 +5286,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T73" s="51" t="n">
+      <c r="T73" s="50" t="n">
         <f aca="false">VLOOKUP(S73,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5312,53 +5312,53 @@
         <f aca="false">+MIN('bid input'!D5,'bid input'!M5)</f>
         <v>1500000</v>
       </c>
-      <c r="F74" s="46" t="n">
+      <c r="F74" s="45" t="n">
         <f aca="false">+IF(D74&gt;0,E74,0)</f>
         <v>0</v>
       </c>
-      <c r="G74" s="47" t="n">
+      <c r="G74" s="46" t="n">
         <f aca="false">+IF($F74&gt;0,RANK($D74,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H74" s="48" t="n">
+      <c r="H74" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B74,$J$96:$K$115,2,0)),0,VLOOKUP(B74,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I74" s="48" t="n">
+      <c r="I74" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B74,$J$96:$K$115,2,0)),0,VLOOKUP(B74,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J74" s="49" t="n">
+      <c r="J74" s="48" t="n">
         <f aca="false">VLOOKUP(B74,'bid input'!B:S,18,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="K74" s="47" t="str">
+      <c r="K74" s="46" t="str">
         <f aca="false">IF(G74=0,"",G74)</f>
         <v/>
       </c>
-      <c r="L74" s="47" t="n">
+      <c r="L74" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K74,K$71:K$90,1)),0,RANK(K74,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M74" s="50" t="n">
+      <c r="M74" s="49" t="n">
         <f aca="false">VALUE(L74&amp;J74)</f>
         <v>40928.625</v>
       </c>
-      <c r="N74" s="47" t="n">
+      <c r="N74" s="46" t="n">
         <f aca="false">IF(L74=0,0,COUNT(M$71:M$90)-(RANK(M74,M$71:M$90,0)+COUNTIF(M$71:M74,M74))+2)</f>
         <v>0</v>
       </c>
-      <c r="O74" s="51" t="inlineStr">
+      <c r="O74" s="50" t="inlineStr">
         <f aca="false">D74</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P74" s="52" t="n">
+      <c r="P74" s="51" t="n">
         <f aca="false">B74</f>
         <v>1104152</v>
       </c>
-      <c r="Q74" s="53"/>
+      <c r="Q74" s="52"/>
       <c r="R74" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5367,7 +5367,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T74" s="51" t="n">
+      <c r="T74" s="50" t="n">
         <f aca="false">VLOOKUP(S74,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5393,53 +5393,53 @@
         <f aca="false">+MIN('bid input'!D6,'bid input'!M6)</f>
         <v>860000</v>
       </c>
-      <c r="F75" s="46" t="n">
+      <c r="F75" s="45" t="n">
         <f aca="false">+IF(D75&gt;0,E75,0)</f>
         <v>0</v>
       </c>
-      <c r="G75" s="47" t="n">
+      <c r="G75" s="46" t="n">
         <f aca="false">+IF($F75&gt;0,RANK($D75,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H75" s="48" t="n">
+      <c r="H75" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B75,$J$96:$K$115,2,0)),0,VLOOKUP(B75,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I75" s="48" t="n">
+      <c r="I75" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B75,$J$96:$K$115,2,0)),0,VLOOKUP(B75,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J75" s="49" t="n">
+      <c r="J75" s="48" t="n">
         <f aca="false">VLOOKUP(B75,'bid input'!B:S,18,0)</f>
         <v>40928.7126388889</v>
       </c>
-      <c r="K75" s="47" t="str">
+      <c r="K75" s="46" t="str">
         <f aca="false">IF(G75=0,"",G75)</f>
         <v/>
       </c>
-      <c r="L75" s="47" t="n">
+      <c r="L75" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K75,K$71:K$90,1)),0,RANK(K75,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M75" s="50" t="n">
+      <c r="M75" s="49" t="n">
         <f aca="false">VALUE(L75&amp;J75)</f>
         <v>40928.7126388889</v>
       </c>
-      <c r="N75" s="47" t="n">
+      <c r="N75" s="46" t="n">
         <f aca="false">IF(L75=0,0,COUNT(M$71:M$90)-(RANK(M75,M$71:M$90,0)+COUNTIF(M$71:M75,M75))+2)</f>
         <v>0</v>
       </c>
-      <c r="O75" s="51" t="inlineStr">
+      <c r="O75" s="50" t="inlineStr">
         <f aca="false">D75</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P75" s="52" t="n">
+      <c r="P75" s="51" t="n">
         <f aca="false">B75</f>
         <v>1104136</v>
       </c>
-      <c r="Q75" s="53"/>
+      <c r="Q75" s="52"/>
       <c r="R75" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5448,7 +5448,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T75" s="51" t="n">
+      <c r="T75" s="50" t="n">
         <f aca="false">VLOOKUP(S75,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5474,53 +5474,53 @@
         <f aca="false">+MIN('bid input'!D7,'bid input'!M7)</f>
         <v>300000</v>
       </c>
-      <c r="F76" s="46" t="n">
+      <c r="F76" s="45" t="n">
         <f aca="false">+IF(D76&gt;0,E76,0)</f>
         <v>0</v>
       </c>
-      <c r="G76" s="47" t="n">
+      <c r="G76" s="46" t="n">
         <f aca="false">+IF($F76&gt;0,RANK($D76,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H76" s="48" t="n">
+      <c r="H76" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B76,$J$96:$K$115,2,0)),0,VLOOKUP(B76,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I76" s="48" t="n">
+      <c r="I76" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B76,$J$96:$K$115,2,0)),0,VLOOKUP(B76,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J76" s="49" t="n">
+      <c r="J76" s="48" t="n">
         <f aca="false">VLOOKUP(B76,'bid input'!B:S,18,0)</f>
         <v>40928.7726388889</v>
       </c>
-      <c r="K76" s="47" t="str">
+      <c r="K76" s="46" t="str">
         <f aca="false">IF(G76=0,"",G76)</f>
         <v/>
       </c>
-      <c r="L76" s="47" t="n">
+      <c r="L76" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K76,K$71:K$90,1)),0,RANK(K76,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M76" s="50" t="n">
+      <c r="M76" s="49" t="n">
         <f aca="false">VALUE(L76&amp;J76)</f>
         <v>40928.7726388889</v>
       </c>
-      <c r="N76" s="47" t="n">
+      <c r="N76" s="46" t="n">
         <f aca="false">IF(L76=0,0,COUNT(M$71:M$90)-(RANK(M76,M$71:M$90,0)+COUNTIF(M$71:M76,M76))+2)</f>
         <v>0</v>
       </c>
-      <c r="O76" s="51" t="inlineStr">
+      <c r="O76" s="50" t="inlineStr">
         <f aca="false">D76</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P76" s="52" t="n">
+      <c r="P76" s="51" t="n">
         <f aca="false">B76</f>
         <v>1104138</v>
       </c>
-      <c r="Q76" s="53"/>
+      <c r="Q76" s="52"/>
       <c r="R76" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T76" s="51" t="n">
+      <c r="T76" s="50" t="n">
         <f aca="false">VLOOKUP(S76,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5555,53 +5555,53 @@
         <f aca="false">+MIN('bid input'!D8,'bid input'!M8)</f>
         <v>250000</v>
       </c>
-      <c r="F77" s="46" t="n">
+      <c r="F77" s="45" t="n">
         <f aca="false">+IF(D77&gt;0,E77,0)</f>
         <v>0</v>
       </c>
-      <c r="G77" s="47" t="n">
+      <c r="G77" s="46" t="n">
         <f aca="false">+IF($F77&gt;0,RANK($D77,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H77" s="48" t="n">
+      <c r="H77" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B77,$J$96:$K$115,2,0)),0,VLOOKUP(B77,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I77" s="48" t="n">
+      <c r="I77" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B77,$J$96:$K$115,2,0)),0,VLOOKUP(B77,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J77" s="49" t="n">
+      <c r="J77" s="48" t="n">
         <f aca="false">VLOOKUP(B77,'bid input'!B:S,18,0)</f>
         <v>40928.8026388889</v>
       </c>
-      <c r="K77" s="47" t="str">
+      <c r="K77" s="46" t="str">
         <f aca="false">IF(G77=0,"",G77)</f>
         <v/>
       </c>
-      <c r="L77" s="47" t="n">
+      <c r="L77" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K77,K$71:K$90,1)),0,RANK(K77,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M77" s="50" t="n">
+      <c r="M77" s="49" t="n">
         <f aca="false">VALUE(L77&amp;J77)</f>
         <v>40928.8026388889</v>
       </c>
-      <c r="N77" s="47" t="n">
+      <c r="N77" s="46" t="n">
         <f aca="false">IF(L77=0,0,COUNT(M$71:M$90)-(RANK(M77,M$71:M$90,0)+COUNTIF(M$71:M77,M77))+2)</f>
         <v>0</v>
       </c>
-      <c r="O77" s="51" t="inlineStr">
+      <c r="O77" s="50" t="inlineStr">
         <f aca="false">D77</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P77" s="52" t="n">
+      <c r="P77" s="51" t="n">
         <f aca="false">B77</f>
         <v>1104139</v>
       </c>
-      <c r="Q77" s="53"/>
+      <c r="Q77" s="52"/>
       <c r="R77" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5610,7 +5610,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T77" s="51" t="n">
+      <c r="T77" s="50" t="n">
         <f aca="false">VLOOKUP(S77,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5636,53 +5636,53 @@
         <f aca="false">+MIN('bid input'!D9,'bid input'!M9)</f>
         <v>74000</v>
       </c>
-      <c r="F78" s="46" t="n">
+      <c r="F78" s="45" t="n">
         <f aca="false">+IF(D78&gt;0,E78,0)</f>
         <v>0</v>
       </c>
-      <c r="G78" s="47" t="n">
+      <c r="G78" s="46" t="n">
         <f aca="false">+IF($F78&gt;0,RANK($D78,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H78" s="48" t="n">
+      <c r="H78" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B78,$J$96:$K$115,2,0)),0,VLOOKUP(B78,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I78" s="48" t="n">
+      <c r="I78" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B78,$J$96:$K$115,2,0)),0,VLOOKUP(B78,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J78" s="49" t="n">
+      <c r="J78" s="48" t="n">
         <f aca="false">VLOOKUP(B78,'bid input'!B:S,18,0)</f>
         <v>40928.8326388889</v>
       </c>
-      <c r="K78" s="47" t="str">
+      <c r="K78" s="46" t="str">
         <f aca="false">IF(G78=0,"",G78)</f>
         <v/>
       </c>
-      <c r="L78" s="47" t="n">
+      <c r="L78" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K78,K$71:K$90,1)),0,RANK(K78,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M78" s="50" t="n">
+      <c r="M78" s="49" t="n">
         <f aca="false">VALUE(L78&amp;J78)</f>
         <v>40928.8326388889</v>
       </c>
-      <c r="N78" s="47" t="n">
+      <c r="N78" s="46" t="n">
         <f aca="false">IF(L78=0,0,COUNT(M$71:M$90)-(RANK(M78,M$71:M$90,0)+COUNTIF(M$71:M78,M78))+2)</f>
         <v>0</v>
       </c>
-      <c r="O78" s="51" t="inlineStr">
+      <c r="O78" s="50" t="inlineStr">
         <f aca="false">D78</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P78" s="52" t="n">
+      <c r="P78" s="51" t="n">
         <f aca="false">B78</f>
         <v>1104140</v>
       </c>
-      <c r="Q78" s="53"/>
+      <c r="Q78" s="52"/>
       <c r="R78" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5691,7 +5691,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T78" s="51" t="n">
+      <c r="T78" s="50" t="n">
         <f aca="false">VLOOKUP(S78,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5717,53 +5717,53 @@
         <f aca="false">+MIN('bid input'!D10,'bid input'!M10)</f>
         <v>285000</v>
       </c>
-      <c r="F79" s="46" t="n">
+      <c r="F79" s="45" t="n">
         <f aca="false">+IF(D79&gt;0,E79,0)</f>
         <v>0</v>
       </c>
-      <c r="G79" s="47" t="n">
+      <c r="G79" s="46" t="n">
         <f aca="false">+IF($F79&gt;0,RANK($D79,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H79" s="48" t="n">
+      <c r="H79" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B79,$J$96:$K$115,2,0)),0,VLOOKUP(B79,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I79" s="48" t="n">
+      <c r="I79" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B79,$J$96:$K$115,2,0)),0,VLOOKUP(B79,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J79" s="49" t="n">
+      <c r="J79" s="48" t="n">
         <f aca="false">VLOOKUP(B79,'bid input'!B:S,18,0)</f>
         <v>40928.8626388889</v>
       </c>
-      <c r="K79" s="47" t="str">
+      <c r="K79" s="46" t="str">
         <f aca="false">IF(G79=0,"",G79)</f>
         <v/>
       </c>
-      <c r="L79" s="47" t="n">
+      <c r="L79" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K79,K$71:K$90,1)),0,RANK(K79,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M79" s="50" t="n">
+      <c r="M79" s="49" t="n">
         <f aca="false">VALUE(L79&amp;J79)</f>
         <v>40928.8626388889</v>
       </c>
-      <c r="N79" s="47" t="n">
+      <c r="N79" s="46" t="n">
         <f aca="false">IF(L79=0,0,COUNT(M$71:M$90)-(RANK(M79,M$71:M$90,0)+COUNTIF(M$71:M79,M79))+2)</f>
         <v>0</v>
       </c>
-      <c r="O79" s="51" t="inlineStr">
+      <c r="O79" s="50" t="inlineStr">
         <f aca="false">D79</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P79" s="52" t="n">
+      <c r="P79" s="51" t="n">
         <f aca="false">B79</f>
         <v>1104141</v>
       </c>
-      <c r="Q79" s="53"/>
+      <c r="Q79" s="52"/>
       <c r="R79" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
@@ -5772,7 +5772,7 @@
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T79" s="51" t="n">
+      <c r="T79" s="50" t="n">
         <f aca="false">VLOOKUP(S79,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
@@ -5798,66 +5798,66 @@
         <f aca="false">+MIN('bid input'!D11,'bid input'!M11)</f>
         <v>532000</v>
       </c>
-      <c r="F80" s="46" t="n">
+      <c r="F80" s="45" t="n">
         <f aca="false">+IF(D80&gt;0,E80,0)</f>
         <v>0</v>
       </c>
-      <c r="G80" s="47" t="n">
+      <c r="G80" s="46" t="n">
         <f aca="false">+IF($F80&gt;0,RANK($D80,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H80" s="48" t="n">
+      <c r="H80" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B80,$J$96:$K$115,2,0)),0,VLOOKUP(B80,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I80" s="48" t="n">
+      <c r="I80" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B80,$J$96:$K$115,2,0)),0,VLOOKUP(B80,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J80" s="49" t="n">
+      <c r="J80" s="48" t="n">
         <f aca="false">VLOOKUP(B80,'bid input'!B:S,18,0)</f>
         <v>40928.9026388889</v>
       </c>
-      <c r="K80" s="47" t="str">
+      <c r="K80" s="46" t="str">
         <f aca="false">IF(G80=0,"",G80)</f>
         <v/>
       </c>
-      <c r="L80" s="47" t="n">
+      <c r="L80" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K80,K$71:K$90,1)),0,RANK(K80,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M80" s="50" t="n">
+      <c r="M80" s="49" t="n">
         <f aca="false">VALUE(L80&amp;J80)</f>
         <v>40928.9026388889</v>
       </c>
-      <c r="N80" s="47" t="n">
+      <c r="N80" s="46" t="n">
         <f aca="false">IF(L80=0,0,COUNT(M$71:M$90)-(RANK(M80,M$71:M$90,0)+COUNTIF(M$71:M80,M80))+2)</f>
         <v>0</v>
       </c>
-      <c r="O80" s="51" t="inlineStr">
+      <c r="O80" s="50" t="inlineStr">
         <f aca="false">D80</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P80" s="52" t="n">
+      <c r="P80" s="51" t="n">
         <f aca="false">B80</f>
         <v>1104159</v>
       </c>
-      <c r="Q80" s="53"/>
+      <c r="Q80" s="52"/>
       <c r="R80" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S80" s="54" t="n">
+      <c r="S80" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T80" s="51" t="n">
+      <c r="T80" s="50" t="n">
         <f aca="false">VLOOKUP(S80,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U80" s="54" t="n">
+      <c r="U80" s="53" t="n">
         <f aca="false">VLOOKUP(S80,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -5879,66 +5879,66 @@
         <f aca="false">+MIN('bid input'!D12,'bid input'!M12)</f>
         <v>292000</v>
       </c>
-      <c r="F81" s="46" t="n">
+      <c r="F81" s="45" t="n">
         <f aca="false">+IF(D81&gt;0,E81,0)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="47" t="n">
+      <c r="G81" s="46" t="n">
         <f aca="false">+IF($F81&gt;0,RANK($D81,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H81" s="48" t="n">
+      <c r="H81" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B81,$J$96:$K$115,2,0)),0,VLOOKUP(B81,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I81" s="48" t="n">
+      <c r="I81" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B81,$J$96:$K$115,2,0)),0,VLOOKUP(B81,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J81" s="49" t="n">
+      <c r="J81" s="48" t="n">
         <f aca="false">VLOOKUP(B81,'bid input'!B:S,18,0)</f>
         <v>40928.9626388889</v>
       </c>
-      <c r="K81" s="47" t="str">
+      <c r="K81" s="46" t="str">
         <f aca="false">IF(G81=0,"",G81)</f>
         <v/>
       </c>
-      <c r="L81" s="47" t="n">
+      <c r="L81" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K81,K$71:K$90,1)),0,RANK(K81,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M81" s="50" t="n">
+      <c r="M81" s="49" t="n">
         <f aca="false">VALUE(L81&amp;J81)</f>
         <v>40928.9626388889</v>
       </c>
-      <c r="N81" s="47" t="n">
+      <c r="N81" s="46" t="n">
         <f aca="false">IF(L81=0,0,COUNT(M$71:M$90)-(RANK(M81,M$71:M$90,0)+COUNTIF(M$71:M81,M81))+2)</f>
         <v>0</v>
       </c>
-      <c r="O81" s="51" t="inlineStr">
+      <c r="O81" s="50" t="inlineStr">
         <f aca="false">D81</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P81" s="52" t="n">
+      <c r="P81" s="51" t="n">
         <f aca="false">B81</f>
         <v>1104161</v>
       </c>
-      <c r="Q81" s="53"/>
+      <c r="Q81" s="52"/>
       <c r="R81" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S81" s="54" t="n">
+      <c r="S81" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T81" s="51" t="n">
+      <c r="T81" s="50" t="n">
         <f aca="false">VLOOKUP(S81,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U81" s="54" t="n">
+      <c r="U81" s="53" t="n">
         <f aca="false">VLOOKUP(S81,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -5960,66 +5960,66 @@
         <f aca="false">+MIN('bid input'!D13,'bid input'!M13)</f>
         <v>752000</v>
       </c>
-      <c r="F82" s="46" t="n">
+      <c r="F82" s="45" t="n">
         <f aca="false">+IF(D82&gt;0,E82,0)</f>
         <v>0</v>
       </c>
-      <c r="G82" s="47" t="n">
+      <c r="G82" s="46" t="n">
         <f aca="false">+IF($F82&gt;0,RANK($D82,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H82" s="48" t="n">
+      <c r="H82" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B82,$J$96:$K$115,2,0)),0,VLOOKUP(B82,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I82" s="48" t="n">
+      <c r="I82" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B82,$J$96:$K$115,2,0)),0,VLOOKUP(B82,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J82" s="49" t="n">
+      <c r="J82" s="48" t="n">
         <f aca="false">VLOOKUP(B82,'bid input'!B:S,18,0)</f>
         <v>40928.9826388889</v>
       </c>
-      <c r="K82" s="47" t="str">
+      <c r="K82" s="46" t="str">
         <f aca="false">IF(G82=0,"",G82)</f>
         <v/>
       </c>
-      <c r="L82" s="47" t="n">
+      <c r="L82" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K82,K$71:K$90,1)),0,RANK(K82,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M82" s="50" t="n">
+      <c r="M82" s="49" t="n">
         <f aca="false">VALUE(L82&amp;J82)</f>
         <v>40928.9826388889</v>
       </c>
-      <c r="N82" s="47" t="n">
+      <c r="N82" s="46" t="n">
         <f aca="false">IF(L82=0,0,COUNT(M$71:M$90)-(RANK(M82,M$71:M$90,0)+COUNTIF(M$71:M82,M82))+2)</f>
         <v>0</v>
       </c>
-      <c r="O82" s="51" t="inlineStr">
+      <c r="O82" s="50" t="inlineStr">
         <f aca="false">D82</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P82" s="52" t="n">
+      <c r="P82" s="51" t="n">
         <f aca="false">B82</f>
         <v>1104145</v>
       </c>
-      <c r="Q82" s="53"/>
+      <c r="Q82" s="52"/>
       <c r="R82" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S82" s="54" t="n">
+      <c r="S82" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T82" s="51" t="n">
+      <c r="T82" s="50" t="n">
         <f aca="false">VLOOKUP(S82,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U82" s="54" t="n">
+      <c r="U82" s="53" t="n">
         <f aca="false">VLOOKUP(S82,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6041,66 +6041,66 @@
         <f aca="false">+MIN('bid input'!D14,'bid input'!M14)</f>
         <v>418000</v>
       </c>
-      <c r="F83" s="46" t="n">
+      <c r="F83" s="45" t="n">
         <f aca="false">+IF(D83&gt;0,E83,0)</f>
         <v>0</v>
       </c>
-      <c r="G83" s="47" t="n">
+      <c r="G83" s="46" t="n">
         <f aca="false">+IF($F83&gt;0,RANK($D83,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H83" s="48" t="n">
+      <c r="H83" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B83,$J$96:$K$115,2,0)),0,VLOOKUP(B83,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I83" s="48" t="n">
+      <c r="I83" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B83,$J$96:$K$115,2,0)),0,VLOOKUP(B83,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J83" s="49" t="n">
+      <c r="J83" s="48" t="n">
         <f aca="false">VLOOKUP(B83,'bid input'!B:S,18,0)</f>
         <v>40929.0993055556</v>
       </c>
-      <c r="K83" s="47" t="str">
+      <c r="K83" s="46" t="str">
         <f aca="false">IF(G83=0,"",G83)</f>
         <v/>
       </c>
-      <c r="L83" s="47" t="n">
+      <c r="L83" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K83,K$71:K$90,1)),0,RANK(K83,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M83" s="50" t="n">
+      <c r="M83" s="49" t="n">
         <f aca="false">VALUE(L83&amp;J83)</f>
         <v>40929.0993055556</v>
       </c>
-      <c r="N83" s="47" t="n">
+      <c r="N83" s="46" t="n">
         <f aca="false">IF(L83=0,0,COUNT(M$71:M$90)-(RANK(M83,M$71:M$90,0)+COUNTIF(M$71:M83,M83))+2)</f>
         <v>0</v>
       </c>
-      <c r="O83" s="51" t="inlineStr">
+      <c r="O83" s="50" t="inlineStr">
         <f aca="false">D83</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P83" s="52" t="n">
+      <c r="P83" s="51" t="n">
         <f aca="false">B83</f>
         <v>1104133</v>
       </c>
-      <c r="Q83" s="53"/>
+      <c r="Q83" s="52"/>
       <c r="R83" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S83" s="54" t="n">
+      <c r="S83" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T83" s="51" t="n">
+      <c r="T83" s="50" t="n">
         <f aca="false">VLOOKUP(S83,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U83" s="54" t="n">
+      <c r="U83" s="53" t="n">
         <f aca="false">VLOOKUP(S83,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6122,66 +6122,66 @@
         <f aca="false">+MIN('bid input'!D15,'bid input'!M15)</f>
         <v>47000</v>
       </c>
-      <c r="F84" s="46" t="n">
+      <c r="F84" s="45" t="n">
         <f aca="false">+IF(D84&gt;0,E84,0)</f>
         <v>0</v>
       </c>
-      <c r="G84" s="47" t="n">
+      <c r="G84" s="46" t="n">
         <f aca="false">+IF($F84&gt;0,RANK($D84,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H84" s="48" t="n">
+      <c r="H84" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B84,$J$96:$K$115,2,0)),0,VLOOKUP(B84,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I84" s="48" t="n">
+      <c r="I84" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B84,$J$96:$K$115,2,0)),0,VLOOKUP(B84,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J84" s="49" t="n">
+      <c r="J84" s="48" t="n">
         <f aca="false">VLOOKUP(B84,'bid input'!B:S,18,0)</f>
         <v>40929.1026388889</v>
       </c>
-      <c r="K84" s="47" t="str">
+      <c r="K84" s="46" t="str">
         <f aca="false">IF(G84=0,"",G84)</f>
         <v/>
       </c>
-      <c r="L84" s="47" t="n">
+      <c r="L84" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K84,K$71:K$90,1)),0,RANK(K84,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M84" s="50" t="n">
+      <c r="M84" s="49" t="n">
         <f aca="false">VALUE(L84&amp;J84)</f>
         <v>40929.1026388889</v>
       </c>
-      <c r="N84" s="47" t="n">
+      <c r="N84" s="46" t="n">
         <f aca="false">IF(L84=0,0,COUNT(M$71:M$90)-(RANK(M84,M$71:M$90,0)+COUNTIF(M$71:M84,M84))+2)</f>
         <v>0</v>
       </c>
-      <c r="O84" s="51" t="inlineStr">
+      <c r="O84" s="50" t="inlineStr">
         <f aca="false">D84</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P84" s="52" t="n">
+      <c r="P84" s="51" t="n">
         <f aca="false">B84</f>
         <v>1104149</v>
       </c>
-      <c r="Q84" s="53"/>
+      <c r="Q84" s="52"/>
       <c r="R84" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S84" s="54" t="n">
+      <c r="S84" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T84" s="51" t="n">
+      <c r="T84" s="50" t="n">
         <f aca="false">VLOOKUP(S84,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U84" s="54" t="n">
+      <c r="U84" s="53" t="n">
         <f aca="false">VLOOKUP(S84,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6203,66 +6203,66 @@
         <f aca="false">+MIN('bid input'!D16,'bid input'!M16)</f>
         <v>283000</v>
       </c>
-      <c r="F85" s="46" t="n">
+      <c r="F85" s="45" t="n">
         <f aca="false">+IF(D85&gt;0,E85,0)</f>
         <v>0</v>
       </c>
-      <c r="G85" s="47" t="n">
+      <c r="G85" s="46" t="n">
         <f aca="false">+IF($F85&gt;0,RANK($D85,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H85" s="48" t="n">
+      <c r="H85" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B85,$J$96:$K$115,2,0)),0,VLOOKUP(B85,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I85" s="48" t="n">
+      <c r="I85" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B85,$J$96:$K$115,2,0)),0,VLOOKUP(B85,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J85" s="49" t="n">
+      <c r="J85" s="48" t="n">
         <f aca="false">VLOOKUP(B85,'bid input'!B:S,18,0)</f>
         <v>40929.1626388889</v>
       </c>
-      <c r="K85" s="47" t="str">
+      <c r="K85" s="46" t="str">
         <f aca="false">IF(G85=0,"",G85)</f>
         <v/>
       </c>
-      <c r="L85" s="47" t="n">
+      <c r="L85" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K85,K$71:K$90,1)),0,RANK(K85,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M85" s="50" t="n">
+      <c r="M85" s="49" t="n">
         <f aca="false">VALUE(L85&amp;J85)</f>
         <v>40929.1626388889</v>
       </c>
-      <c r="N85" s="47" t="n">
+      <c r="N85" s="46" t="n">
         <f aca="false">IF(L85=0,0,COUNT(M$71:M$90)-(RANK(M85,M$71:M$90,0)+COUNTIF(M$71:M85,M85))+2)</f>
         <v>0</v>
       </c>
-      <c r="O85" s="51" t="inlineStr">
+      <c r="O85" s="50" t="inlineStr">
         <f aca="false">D85</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P85" s="52" t="n">
+      <c r="P85" s="51" t="n">
         <f aca="false">B85</f>
         <v>1104151</v>
       </c>
-      <c r="Q85" s="53"/>
+      <c r="Q85" s="52"/>
       <c r="R85" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S85" s="54" t="n">
+      <c r="S85" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T85" s="51" t="n">
+      <c r="T85" s="50" t="n">
         <f aca="false">VLOOKUP(S85,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U85" s="54" t="n">
+      <c r="U85" s="53" t="n">
         <f aca="false">VLOOKUP(S85,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6284,66 +6284,66 @@
         <f aca="false">+MIN('bid input'!D17,'bid input'!M17)</f>
         <v>598000</v>
       </c>
-      <c r="F86" s="46" t="n">
+      <c r="F86" s="45" t="n">
         <f aca="false">+IF(D86&gt;0,E86,0)</f>
         <v>0</v>
       </c>
-      <c r="G86" s="47" t="n">
+      <c r="G86" s="46" t="n">
         <f aca="false">+IF($F86&gt;0,RANK($D86,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H86" s="48" t="n">
+      <c r="H86" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B86,$J$96:$K$115,2,0)),0,VLOOKUP(B86,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I86" s="48" t="n">
+      <c r="I86" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B86,$J$96:$K$115,2,0)),0,VLOOKUP(B86,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J86" s="49" t="n">
+      <c r="J86" s="48" t="n">
         <f aca="false">VLOOKUP(B86,'bid input'!B:S,18,0)</f>
         <v>40929.1926388889</v>
       </c>
-      <c r="K86" s="47" t="str">
+      <c r="K86" s="46" t="str">
         <f aca="false">IF(G86=0,"",G86)</f>
         <v/>
       </c>
-      <c r="L86" s="47" t="n">
+      <c r="L86" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K86,K$71:K$90,1)),0,RANK(K86,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M86" s="50" t="n">
+      <c r="M86" s="49" t="n">
         <f aca="false">VALUE(L86&amp;J86)</f>
         <v>40929.1926388889</v>
       </c>
-      <c r="N86" s="47" t="n">
+      <c r="N86" s="46" t="n">
         <f aca="false">IF(L86=0,0,COUNT(M$71:M$90)-(RANK(M86,M$71:M$90,0)+COUNTIF(M$71:M86,M86))+2)</f>
         <v>0</v>
       </c>
-      <c r="O86" s="51" t="inlineStr">
+      <c r="O86" s="50" t="inlineStr">
         <f aca="false">D86</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P86" s="52" t="n">
+      <c r="P86" s="51" t="n">
         <f aca="false">B86</f>
         <v>1104131</v>
       </c>
-      <c r="Q86" s="53"/>
+      <c r="Q86" s="52"/>
       <c r="R86" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S86" s="54" t="n">
+      <c r="S86" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T86" s="51" t="n">
+      <c r="T86" s="50" t="n">
         <f aca="false">VLOOKUP(S86,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U86" s="54" t="n">
+      <c r="U86" s="53" t="n">
         <f aca="false">VLOOKUP(S86,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6365,66 +6365,66 @@
         <f aca="false">+MIN('bid input'!D18,'bid input'!M18)</f>
         <v>639000</v>
       </c>
-      <c r="F87" s="46" t="n">
+      <c r="F87" s="45" t="n">
         <f aca="false">+IF(D87&gt;0,E87,0)</f>
         <v>0</v>
       </c>
-      <c r="G87" s="47" t="n">
+      <c r="G87" s="46" t="n">
         <f aca="false">+IF($F87&gt;0,RANK($D87,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H87" s="48" t="n">
+      <c r="H87" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B87,$J$96:$K$115,2,0)),0,VLOOKUP(B87,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I87" s="48" t="n">
+      <c r="I87" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B87,$J$96:$K$115,2,0)),0,VLOOKUP(B87,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J87" s="49" t="n">
+      <c r="J87" s="48" t="n">
         <f aca="false">VLOOKUP(B87,'bid input'!B:S,18,0)</f>
         <v>40929.2826388889</v>
       </c>
-      <c r="K87" s="47" t="str">
+      <c r="K87" s="46" t="str">
         <f aca="false">IF(G87=0,"",G87)</f>
         <v/>
       </c>
-      <c r="L87" s="47" t="n">
+      <c r="L87" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K87,K$71:K$90,1)),0,RANK(K87,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M87" s="50" t="n">
+      <c r="M87" s="49" t="n">
         <f aca="false">VALUE(L87&amp;J87)</f>
         <v>40929.2826388889</v>
       </c>
-      <c r="N87" s="47" t="n">
+      <c r="N87" s="46" t="n">
         <f aca="false">IF(L87=0,0,COUNT(M$71:M$90)-(RANK(M87,M$71:M$90,0)+COUNTIF(M$71:M87,M87))+2)</f>
         <v>0</v>
       </c>
-      <c r="O87" s="51" t="inlineStr">
+      <c r="O87" s="50" t="inlineStr">
         <f aca="false">D87</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P87" s="52" t="n">
+      <c r="P87" s="51" t="n">
         <f aca="false">B87</f>
         <v>1104155</v>
       </c>
-      <c r="Q87" s="53"/>
+      <c r="Q87" s="52"/>
       <c r="R87" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S87" s="54" t="n">
+      <c r="S87" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T87" s="51" t="n">
+      <c r="T87" s="50" t="n">
         <f aca="false">VLOOKUP(S87,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U87" s="54" t="n">
+      <c r="U87" s="53" t="n">
         <f aca="false">VLOOKUP(S87,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6446,66 +6446,66 @@
         <f aca="false">+MIN('bid input'!D19,'bid input'!M19)</f>
         <v>274000</v>
       </c>
-      <c r="F88" s="46" t="n">
+      <c r="F88" s="45" t="n">
         <f aca="false">+IF(D88&gt;0,E88,0)</f>
         <v>0</v>
       </c>
-      <c r="G88" s="47" t="n">
+      <c r="G88" s="46" t="n">
         <f aca="false">+IF($F88&gt;0,RANK($D88,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H88" s="48" t="n">
+      <c r="H88" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B88,$J$96:$K$115,2,0)),0,VLOOKUP(B88,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I88" s="48" t="n">
+      <c r="I88" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B88,$J$96:$K$115,2,0)),0,VLOOKUP(B88,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J88" s="49" t="n">
+      <c r="J88" s="48" t="n">
         <f aca="false">VLOOKUP(B88,'bid input'!B:S,18,0)</f>
         <v>40929.3126388889</v>
       </c>
-      <c r="K88" s="47" t="str">
+      <c r="K88" s="46" t="str">
         <f aca="false">IF(G88=0,"",G88)</f>
         <v/>
       </c>
-      <c r="L88" s="47" t="n">
+      <c r="L88" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K88,K$71:K$90,1)),0,RANK(K88,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M88" s="50" t="n">
+      <c r="M88" s="49" t="n">
         <f aca="false">VALUE(L88&amp;J88)</f>
         <v>40929.3126388889</v>
       </c>
-      <c r="N88" s="47" t="n">
+      <c r="N88" s="46" t="n">
         <f aca="false">IF(L88=0,0,COUNT(M$71:M$90)-(RANK(M88,M$71:M$90,0)+COUNTIF(M$71:M88,M88))+2)</f>
         <v>0</v>
       </c>
-      <c r="O88" s="51" t="inlineStr">
+      <c r="O88" s="50" t="inlineStr">
         <f aca="false">D88</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P88" s="52" t="n">
+      <c r="P88" s="51" t="n">
         <f aca="false">B88</f>
         <v>1104156</v>
       </c>
-      <c r="Q88" s="53"/>
+      <c r="Q88" s="52"/>
       <c r="R88" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S88" s="54" t="n">
+      <c r="S88" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T88" s="51" t="n">
+      <c r="T88" s="50" t="n">
         <f aca="false">VLOOKUP(S88,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U88" s="54" t="n">
+      <c r="U88" s="53" t="n">
         <f aca="false">VLOOKUP(S88,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6527,66 +6527,66 @@
         <f aca="false">+MIN('bid input'!D20,'bid input'!M20)</f>
         <v>629000</v>
       </c>
-      <c r="F89" s="46" t="n">
+      <c r="F89" s="45" t="n">
         <f aca="false">+IF(D89&gt;0,E89,0)</f>
         <v>0</v>
       </c>
-      <c r="G89" s="47" t="n">
+      <c r="G89" s="46" t="n">
         <f aca="false">+IF($F89&gt;0,RANK($D89,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H89" s="48" t="n">
+      <c r="H89" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B89,$J$96:$K$115,2,0)),0,VLOOKUP(B89,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I89" s="48" t="n">
+      <c r="I89" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B89,$J$96:$K$115,2,0)),0,VLOOKUP(B89,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J89" s="49" t="n">
+      <c r="J89" s="48" t="n">
         <f aca="false">VLOOKUP(B89,'bid input'!B:S,18,0)</f>
         <v>40929.3426388889</v>
       </c>
-      <c r="K89" s="47" t="str">
+      <c r="K89" s="46" t="str">
         <f aca="false">IF(G89=0,"",G89)</f>
         <v/>
       </c>
-      <c r="L89" s="47" t="n">
+      <c r="L89" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K89,K$71:K$90,1)),0,RANK(K89,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M89" s="50" t="n">
+      <c r="M89" s="49" t="n">
         <f aca="false">VALUE(L89&amp;J89)</f>
         <v>40929.3426388889</v>
       </c>
-      <c r="N89" s="47" t="n">
+      <c r="N89" s="46" t="n">
         <f aca="false">IF(L89=0,0,COUNT(M$71:M$90)-(RANK(M89,M$71:M$90,0)+COUNTIF(M$71:M89,M89))+2)</f>
         <v>0</v>
       </c>
-      <c r="O89" s="51" t="inlineStr">
+      <c r="O89" s="50" t="inlineStr">
         <f aca="false">D89</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P89" s="52" t="n">
+      <c r="P89" s="51" t="n">
         <f aca="false">B89</f>
         <v>1104157</v>
       </c>
-      <c r="Q89" s="53"/>
+      <c r="Q89" s="52"/>
       <c r="R89" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S89" s="54" t="n">
+      <c r="S89" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T89" s="51" t="n">
+      <c r="T89" s="50" t="n">
         <f aca="false">VLOOKUP(S89,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U89" s="54" t="n">
+      <c r="U89" s="53" t="n">
         <f aca="false">VLOOKUP(S89,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6608,66 +6608,66 @@
         <f aca="false">+MIN('bid input'!D21,'bid input'!M21)</f>
         <v>562000</v>
       </c>
-      <c r="F90" s="46" t="n">
+      <c r="F90" s="45" t="n">
         <f aca="false">+IF(D90&gt;0,E90,0)</f>
         <v>0</v>
       </c>
-      <c r="G90" s="47" t="n">
+      <c r="G90" s="46" t="n">
         <f aca="false">+IF($F90&gt;0,RANK($D90,$D$71:$D$90,1),0)</f>
         <v>0</v>
       </c>
-      <c r="H90" s="48" t="n">
+      <c r="H90" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B90,$J$96:$K$115,2,0)),0,VLOOKUP(B90,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="I90" s="48" t="n">
+      <c r="I90" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B90,$J$96:$K$115,2,0)),0,VLOOKUP(B90,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
-      <c r="J90" s="49" t="n">
+      <c r="J90" s="48" t="n">
         <f aca="false">VLOOKUP(B90,'bid input'!B:S,18,0)</f>
         <v>40929.3726388889</v>
       </c>
-      <c r="K90" s="47" t="str">
+      <c r="K90" s="46" t="str">
         <f aca="false">IF(G90=0,"",G90)</f>
         <v/>
       </c>
-      <c r="L90" s="47" t="n">
+      <c r="L90" s="46" t="n">
         <f aca="false">IF(ISERROR(RANK(K90,K$71:K$90,1)),0,RANK(K90,K$71:K$90,1))</f>
         <v>0</v>
       </c>
-      <c r="M90" s="50" t="n">
+      <c r="M90" s="49" t="n">
         <f aca="false">VALUE(L90&amp;J90)</f>
         <v>40929.3726388889</v>
       </c>
-      <c r="N90" s="47" t="n">
+      <c r="N90" s="46" t="n">
         <f aca="false">IF(L90=0,0,COUNT(M$71:M$90)-(RANK(M90,M$71:M$90,0)+COUNTIF(M$71:M90,M90))+2)</f>
         <v>0</v>
       </c>
-      <c r="O90" s="51" t="inlineStr">
+      <c r="O90" s="50" t="inlineStr">
         <f aca="false">D90</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="P90" s="52" t="n">
+      <c r="P90" s="51" t="n">
         <f aca="false">B90</f>
         <v>1104158</v>
       </c>
-      <c r="Q90" s="53"/>
+      <c r="Q90" s="52"/>
       <c r="R90" s="1" t="n">
         <f aca="true">OFFSET(N$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="S90" s="54" t="n">
+      <c r="S90" s="53" t="n">
         <f aca="true">OFFSET(M$71,MATCH(SMALL(N$71:N$90,ROW()-ROW(R$71)+1),N$71:N$90,0)-1,0)</f>
         <v>40928.625</v>
       </c>
-      <c r="T90" s="51" t="n">
+      <c r="T90" s="50" t="n">
         <f aca="false">VLOOKUP(S90,M$71:O$90,3,0)</f>
         <v>0</v>
       </c>
-      <c r="U90" s="54" t="n">
+      <c r="U90" s="53" t="n">
         <f aca="false">VLOOKUP(S90,M$71:P$90,4,0)</f>
         <v>1104134</v>
       </c>
@@ -6691,17 +6691,17 @@
       <c r="F91" s="14"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
-      <c r="I91" s="48" t="n">
+      <c r="I91" s="47" t="n">
         <f aca="false">+IF(ISERROR(VLOOKUP(B91,$J$96:$K$115,2,0)),0,VLOOKUP(B91,$J$96:$K$115,2,0))</f>
         <v>0</v>
       </c>
       <c r="J91" s="14"/>
       <c r="K91" s="14"/>
       <c r="L91" s="14"/>
-      <c r="P91" s="55"/>
+      <c r="P91" s="54"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="92">
-      <c r="D92" s="56"/>
+      <c r="D92" s="55"/>
       <c r="I92" s="19" t="n">
         <f aca="false">+IF(ISERR(SUMPRODUCT(D71:D90,I71:I90)/I91),0,SUMPRODUCT(D71:D90,I71:I90)/I91)</f>
         <v>0</v>
@@ -6715,8 +6715,8 @@
         <f aca="false">IF(M62="UNDER",+M61,0)</f>
         <v>936360.5</v>
       </c>
-      <c r="Q93" s="54"/>
-      <c r="R93" s="54"/>
+      <c r="Q93" s="53"/>
+      <c r="R93" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="94">
       <c r="B94" s="0" t="s">
@@ -6731,32 +6731,32 @@
       <c r="J94" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q94" s="54"/>
-      <c r="R94" s="54"/>
+      <c r="Q94" s="53"/>
+      <c r="R94" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="95">
       <c r="E95" s="18"/>
       <c r="F95" s="14"/>
       <c r="H95" s="1"/>
-      <c r="I95" s="57" t="n">
+      <c r="I95" s="56" t="n">
         <f aca="false">E93</f>
         <v>936360.5</v>
       </c>
       <c r="J95" s="1"/>
-      <c r="Q95" s="54"/>
-      <c r="R95" s="54"/>
+      <c r="Q95" s="53"/>
+      <c r="R95" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="96">
-      <c r="E96" s="48"/>
+      <c r="E96" s="47"/>
       <c r="F96" s="18"/>
       <c r="G96" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H96" s="58" t="n">
+      <c r="H96" s="57" t="n">
         <f aca="false">+IF(I95&gt;0,MIN(SUMIF($N$71:$N$90,G96,$E$71:$E$90),I95),0)</f>
         <v>0</v>
       </c>
-      <c r="I96" s="57" t="n">
+      <c r="I96" s="56" t="n">
         <f aca="false">I95-H96</f>
         <v>936360.5</v>
       </c>
@@ -6768,21 +6768,21 @@
         <f aca="false">+H96</f>
         <v>0</v>
       </c>
-      <c r="Q96" s="54"/>
-      <c r="R96" s="54"/>
+      <c r="Q96" s="53"/>
+      <c r="R96" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="97">
-      <c r="E97" s="48"/>
+      <c r="E97" s="47"/>
       <c r="F97" s="18"/>
       <c r="G97" s="1" t="n">
         <f aca="false">1+G96</f>
         <v>2</v>
       </c>
-      <c r="H97" s="58" t="n">
+      <c r="H97" s="57" t="n">
         <f aca="false">+IF(I96&gt;0,MIN(SUMIF($N$71:$N$90,G97,$E$71:$E$90),I96),0)</f>
         <v>0</v>
       </c>
-      <c r="I97" s="57" t="n">
+      <c r="I97" s="56" t="n">
         <f aca="false">I96-H97</f>
         <v>936360.5</v>
       </c>
@@ -6794,21 +6794,21 @@
         <f aca="false">+H97</f>
         <v>0</v>
       </c>
-      <c r="Q97" s="54"/>
-      <c r="R97" s="54"/>
+      <c r="Q97" s="53"/>
+      <c r="R97" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="98">
-      <c r="E98" s="48"/>
+      <c r="E98" s="47"/>
       <c r="F98" s="18"/>
       <c r="G98" s="1" t="n">
         <f aca="false">1+G97</f>
         <v>3</v>
       </c>
-      <c r="H98" s="58" t="n">
+      <c r="H98" s="57" t="n">
         <f aca="false">+IF(I97&gt;0,MIN(SUMIF($N$71:$N$90,G98,$E$71:$E$90),I97),0)</f>
         <v>0</v>
       </c>
-      <c r="I98" s="57" t="n">
+      <c r="I98" s="56" t="n">
         <f aca="false">I97-H98</f>
         <v>936360.5</v>
       </c>
@@ -6820,21 +6820,21 @@
         <f aca="false">+H98</f>
         <v>0</v>
       </c>
-      <c r="Q98" s="54"/>
-      <c r="R98" s="54"/>
+      <c r="Q98" s="53"/>
+      <c r="R98" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="99">
-      <c r="E99" s="48"/>
+      <c r="E99" s="47"/>
       <c r="F99" s="18"/>
       <c r="G99" s="1" t="n">
         <f aca="false">1+G98</f>
         <v>4</v>
       </c>
-      <c r="H99" s="58" t="n">
+      <c r="H99" s="57" t="n">
         <f aca="false">+IF(I98&gt;0,MIN(SUMIF($N$71:$N$90,G99,$E$71:$E$90),I98),0)</f>
         <v>0</v>
       </c>
-      <c r="I99" s="57" t="n">
+      <c r="I99" s="56" t="n">
         <f aca="false">I98-H99</f>
         <v>936360.5</v>
       </c>
@@ -6846,21 +6846,21 @@
         <f aca="false">+H99</f>
         <v>0</v>
       </c>
-      <c r="Q99" s="54"/>
-      <c r="R99" s="54"/>
+      <c r="Q99" s="53"/>
+      <c r="R99" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="100">
-      <c r="E100" s="48"/>
+      <c r="E100" s="47"/>
       <c r="F100" s="18"/>
       <c r="G100" s="1" t="n">
         <f aca="false">1+G99</f>
         <v>5</v>
       </c>
-      <c r="H100" s="58" t="n">
+      <c r="H100" s="57" t="n">
         <f aca="false">+IF(I99&gt;0,MIN(SUMIF($N$71:$N$90,G100,$E$71:$E$90),I99),0)</f>
         <v>0</v>
       </c>
-      <c r="I100" s="57" t="n">
+      <c r="I100" s="56" t="n">
         <f aca="false">I99-H100</f>
         <v>936360.5</v>
       </c>
@@ -6872,21 +6872,21 @@
         <f aca="false">+H100</f>
         <v>0</v>
       </c>
-      <c r="Q100" s="54"/>
-      <c r="R100" s="54"/>
+      <c r="Q100" s="53"/>
+      <c r="R100" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="101">
-      <c r="E101" s="48"/>
+      <c r="E101" s="47"/>
       <c r="F101" s="18"/>
       <c r="G101" s="1" t="n">
         <f aca="false">1+G100</f>
         <v>6</v>
       </c>
-      <c r="H101" s="58" t="n">
+      <c r="H101" s="57" t="n">
         <f aca="false">+IF(I100&gt;0,MIN(SUMIF($N$71:$N$90,G101,$E$71:$E$90),I100),0)</f>
         <v>0</v>
       </c>
-      <c r="I101" s="57" t="n">
+      <c r="I101" s="56" t="n">
         <f aca="false">I100-H101</f>
         <v>936360.5</v>
       </c>
@@ -6898,21 +6898,21 @@
         <f aca="false">+H101</f>
         <v>0</v>
       </c>
-      <c r="Q101" s="54"/>
-      <c r="R101" s="54"/>
+      <c r="Q101" s="53"/>
+      <c r="R101" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="102">
-      <c r="E102" s="48"/>
+      <c r="E102" s="47"/>
       <c r="F102" s="18"/>
       <c r="G102" s="1" t="n">
         <f aca="false">1+G101</f>
         <v>7</v>
       </c>
-      <c r="H102" s="58" t="n">
+      <c r="H102" s="57" t="n">
         <f aca="false">+IF(I101&gt;0,MIN(SUMIF($N$71:$N$90,G102,$E$71:$E$90),I101),0)</f>
         <v>0</v>
       </c>
-      <c r="I102" s="57" t="n">
+      <c r="I102" s="56" t="n">
         <f aca="false">I101-H102</f>
         <v>936360.5</v>
       </c>
@@ -6924,21 +6924,21 @@
         <f aca="false">+H102</f>
         <v>0</v>
       </c>
-      <c r="Q102" s="54"/>
-      <c r="R102" s="54"/>
+      <c r="Q102" s="53"/>
+      <c r="R102" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="103">
-      <c r="E103" s="48"/>
+      <c r="E103" s="47"/>
       <c r="F103" s="18"/>
       <c r="G103" s="1" t="n">
         <f aca="false">1+G102</f>
         <v>8</v>
       </c>
-      <c r="H103" s="58" t="n">
+      <c r="H103" s="57" t="n">
         <f aca="false">+IF(I102&gt;0,MIN(SUMIF($N$71:$N$90,G103,$E$71:$E$90),I102),0)</f>
         <v>0</v>
       </c>
-      <c r="I103" s="57" t="n">
+      <c r="I103" s="56" t="n">
         <f aca="false">I102-H103</f>
         <v>936360.5</v>
       </c>
@@ -6950,21 +6950,21 @@
         <f aca="false">+H103</f>
         <v>0</v>
       </c>
-      <c r="Q103" s="54"/>
-      <c r="R103" s="54"/>
+      <c r="Q103" s="53"/>
+      <c r="R103" s="53"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="104">
-      <c r="E104" s="48"/>
+      <c r="E104" s="47"/>
       <c r="F104" s="18"/>
       <c r="G104" s="1" t="n">
         <f aca="false">1+G103</f>
         <v>9</v>
       </c>
-      <c r="H104" s="58" t="n">
+      <c r="H104" s="57" t="n">
         <f aca="false">+IF(I103&gt;0,MIN(SUMIF($N$71:$N$90,G104,$E$71:$E$90),I103),0)</f>
         <v>0</v>
       </c>
-      <c r="I104" s="57" t="n">
+      <c r="I104" s="56" t="n">
         <f aca="false">I103-H104</f>
         <v>936360.5</v>
       </c>
@@ -6978,17 +6978,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="105">
-      <c r="E105" s="48"/>
+      <c r="E105" s="47"/>
       <c r="F105" s="18"/>
       <c r="G105" s="1" t="n">
         <f aca="false">1+G104</f>
         <v>10</v>
       </c>
-      <c r="H105" s="58" t="n">
+      <c r="H105" s="57" t="n">
         <f aca="false">+IF(I104&gt;0,MIN(SUMIF($N$71:$N$90,G105,$E$71:$E$90),I104),0)</f>
         <v>0</v>
       </c>
-      <c r="I105" s="57" t="n">
+      <c r="I105" s="56" t="n">
         <f aca="false">I104-H105</f>
         <v>936360.5</v>
       </c>
@@ -7002,17 +7002,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="106">
-      <c r="E106" s="48"/>
+      <c r="E106" s="47"/>
       <c r="F106" s="18"/>
       <c r="G106" s="1" t="n">
         <f aca="false">1+G105</f>
         <v>11</v>
       </c>
-      <c r="H106" s="58" t="n">
+      <c r="H106" s="57" t="n">
         <f aca="false">+IF(I105&gt;0,MIN(SUMIF($N$71:$N$90,G106,$E$71:$E$90),I105),0)</f>
         <v>0</v>
       </c>
-      <c r="I106" s="57" t="n">
+      <c r="I106" s="56" t="n">
         <f aca="false">I105-H106</f>
         <v>936360.5</v>
       </c>
@@ -7026,17 +7026,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="107">
-      <c r="E107" s="48"/>
+      <c r="E107" s="47"/>
       <c r="F107" s="18"/>
       <c r="G107" s="1" t="n">
         <f aca="false">1+G106</f>
         <v>12</v>
       </c>
-      <c r="H107" s="58" t="n">
+      <c r="H107" s="57" t="n">
         <f aca="false">+IF(I106&gt;0,MIN(SUMIF($N$71:$N$90,G107,$E$71:$E$90),I106),0)</f>
         <v>0</v>
       </c>
-      <c r="I107" s="57" t="n">
+      <c r="I107" s="56" t="n">
         <f aca="false">I106-H107</f>
         <v>936360.5</v>
       </c>
@@ -7050,17 +7050,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="108">
-      <c r="E108" s="48"/>
+      <c r="E108" s="47"/>
       <c r="F108" s="18"/>
       <c r="G108" s="1" t="n">
         <f aca="false">1+G107</f>
         <v>13</v>
       </c>
-      <c r="H108" s="58" t="n">
+      <c r="H108" s="57" t="n">
         <f aca="false">+IF(I107&gt;0,MIN(SUMIF($N$71:$N$90,G108,$E$71:$E$90),I107),0)</f>
         <v>0</v>
       </c>
-      <c r="I108" s="57" t="n">
+      <c r="I108" s="56" t="n">
         <f aca="false">I107-H108</f>
         <v>936360.5</v>
       </c>
@@ -7074,17 +7074,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="109">
-      <c r="E109" s="48"/>
+      <c r="E109" s="47"/>
       <c r="F109" s="18"/>
       <c r="G109" s="1" t="n">
         <f aca="false">1+G108</f>
         <v>14</v>
       </c>
-      <c r="H109" s="58" t="n">
+      <c r="H109" s="57" t="n">
         <f aca="false">+IF(I108&gt;0,MIN(SUMIF($N$71:$N$90,G109,$E$71:$E$90),I108),0)</f>
         <v>0</v>
       </c>
-      <c r="I109" s="57" t="n">
+      <c r="I109" s="56" t="n">
         <f aca="false">I108-H109</f>
         <v>936360.5</v>
       </c>
@@ -7098,17 +7098,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="110">
-      <c r="E110" s="48"/>
+      <c r="E110" s="47"/>
       <c r="F110" s="18"/>
       <c r="G110" s="1" t="n">
         <f aca="false">1+G109</f>
         <v>15</v>
       </c>
-      <c r="H110" s="58" t="n">
+      <c r="H110" s="57" t="n">
         <f aca="false">+IF(I109&gt;0,MIN(SUMIF($N$71:$N$90,G110,$E$71:$E$90),I109),0)</f>
         <v>0</v>
       </c>
-      <c r="I110" s="57" t="n">
+      <c r="I110" s="56" t="n">
         <f aca="false">I109-H110</f>
         <v>936360.5</v>
       </c>
@@ -7122,17 +7122,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="111">
-      <c r="E111" s="48"/>
+      <c r="E111" s="47"/>
       <c r="F111" s="18"/>
       <c r="G111" s="1" t="n">
         <f aca="false">1+G110</f>
         <v>16</v>
       </c>
-      <c r="H111" s="58" t="n">
+      <c r="H111" s="57" t="n">
         <f aca="false">+IF(I110&gt;0,MIN(SUMIF($N$71:$N$90,G111,$E$71:$E$90),I110),0)</f>
         <v>0</v>
       </c>
-      <c r="I111" s="57" t="n">
+      <c r="I111" s="56" t="n">
         <f aca="false">I110-H111</f>
         <v>936360.5</v>
       </c>
@@ -7146,17 +7146,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="112">
-      <c r="E112" s="48"/>
+      <c r="E112" s="47"/>
       <c r="F112" s="18"/>
       <c r="G112" s="1" t="n">
         <f aca="false">1+G111</f>
         <v>17</v>
       </c>
-      <c r="H112" s="58" t="n">
+      <c r="H112" s="57" t="n">
         <f aca="false">+IF(I111&gt;0,MIN(SUMIF($N$71:$N$90,G112,$E$71:$E$90),I111),0)</f>
         <v>0</v>
       </c>
-      <c r="I112" s="57" t="n">
+      <c r="I112" s="56" t="n">
         <f aca="false">I111-H112</f>
         <v>936360.5</v>
       </c>
@@ -7170,17 +7170,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="113">
-      <c r="E113" s="48"/>
+      <c r="E113" s="47"/>
       <c r="F113" s="18"/>
       <c r="G113" s="1" t="n">
         <f aca="false">1+G112</f>
         <v>18</v>
       </c>
-      <c r="H113" s="58" t="n">
+      <c r="H113" s="57" t="n">
         <f aca="false">+IF(I112&gt;0,MIN(SUMIF($N$71:$N$90,G113,$E$71:$E$90),I112),0)</f>
         <v>0</v>
       </c>
-      <c r="I113" s="57" t="n">
+      <c r="I113" s="56" t="n">
         <f aca="false">I112-H113</f>
         <v>936360.5</v>
       </c>
@@ -7194,17 +7194,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="114">
-      <c r="E114" s="48"/>
+      <c r="E114" s="47"/>
       <c r="F114" s="18"/>
       <c r="G114" s="1" t="n">
         <f aca="false">1+G113</f>
         <v>19</v>
       </c>
-      <c r="H114" s="58" t="n">
+      <c r="H114" s="57" t="n">
         <f aca="false">+IF(I113&gt;0,MIN(SUMIF($N$71:$N$90,G114,$E$71:$E$90),I113),0)</f>
         <v>0</v>
       </c>
-      <c r="I114" s="57" t="n">
+      <c r="I114" s="56" t="n">
         <f aca="false">I113-H114</f>
         <v>936360.5</v>
       </c>
@@ -7218,17 +7218,17 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="115">
-      <c r="E115" s="48"/>
+      <c r="E115" s="47"/>
       <c r="F115" s="18"/>
       <c r="G115" s="1" t="n">
         <f aca="false">1+G114</f>
         <v>20</v>
       </c>
-      <c r="H115" s="58" t="n">
+      <c r="H115" s="57" t="n">
         <f aca="false">+IF(I114&gt;0,MIN(SUMIF($N$71:$N$90,G115,$E$71:$E$90),I114),0)</f>
         <v>0</v>
       </c>
-      <c r="I115" s="57" t="n">
+      <c r="I115" s="56" t="n">
         <f aca="false">I114-H115</f>
         <v>936360.5</v>
       </c>
@@ -7294,7 +7294,7 @@
         <f aca="false">+B71</f>
         <v>1104134</v>
       </c>
-      <c r="C119" s="59" t="inlineStr">
+      <c r="C119" s="58" t="inlineStr">
         <f aca="false">+D71</f>
         <is>
           <t/>
@@ -7304,31 +7304,31 @@
         <f aca="false">+I71</f>
         <v>0</v>
       </c>
-      <c r="E119" s="59" t="n">
+      <c r="E119" s="58" t="n">
         <f aca="false">+IF(D119&gt;0,C119+(SUMPRODUCT($G119:$L119,$G$141:$L$141)/$M119),0)</f>
         <v>0</v>
       </c>
-      <c r="G119" s="48" t="n">
+      <c r="G119" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D119</f>
         <v>0</v>
       </c>
-      <c r="H119" s="48" t="n">
+      <c r="H119" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D119</f>
         <v>-0</v>
       </c>
-      <c r="I119" s="48" t="n">
+      <c r="I119" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D119</f>
         <v>0</v>
       </c>
-      <c r="J119" s="48" t="n">
+      <c r="J119" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D119</f>
         <v>0</v>
       </c>
-      <c r="K119" s="48" t="n">
+      <c r="K119" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D119</f>
         <v>0</v>
       </c>
-      <c r="L119" s="48" t="n">
+      <c r="L119" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D119</f>
         <v>0</v>
       </c>
@@ -7342,7 +7342,7 @@
         <f aca="false">+B72</f>
         <v>1104143</v>
       </c>
-      <c r="C120" s="59" t="inlineStr">
+      <c r="C120" s="58" t="inlineStr">
         <f aca="false">+D72</f>
         <is>
           <t/>
@@ -7352,31 +7352,31 @@
         <f aca="false">+I72</f>
         <v>0</v>
       </c>
-      <c r="E120" s="59" t="n">
+      <c r="E120" s="58" t="n">
         <f aca="false">+IF(D120&gt;0,C120+(SUMPRODUCT($G120:$L120,$G$141:$L$141)/$M120),0)</f>
         <v>0</v>
       </c>
-      <c r="G120" s="48" t="n">
+      <c r="G120" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D120</f>
         <v>0</v>
       </c>
-      <c r="H120" s="48" t="n">
+      <c r="H120" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D120</f>
         <v>-0</v>
       </c>
-      <c r="I120" s="48" t="n">
+      <c r="I120" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D120</f>
         <v>0</v>
       </c>
-      <c r="J120" s="48" t="n">
+      <c r="J120" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D120</f>
         <v>0</v>
       </c>
-      <c r="K120" s="48" t="n">
+      <c r="K120" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D120</f>
         <v>0</v>
       </c>
-      <c r="L120" s="48" t="n">
+      <c r="L120" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D120</f>
         <v>0</v>
       </c>
@@ -7390,7 +7390,7 @@
         <f aca="false">+B73</f>
         <v>1104154</v>
       </c>
-      <c r="C121" s="59" t="inlineStr">
+      <c r="C121" s="58" t="inlineStr">
         <f aca="false">+D73</f>
         <is>
           <t/>
@@ -7400,31 +7400,31 @@
         <f aca="false">+I73</f>
         <v>0</v>
       </c>
-      <c r="E121" s="59" t="n">
+      <c r="E121" s="58" t="n">
         <f aca="false">+IF(D121&gt;0,C121+(SUMPRODUCT($G121:$L121,$G$141:$L$141)/$M121),0)</f>
         <v>0</v>
       </c>
-      <c r="G121" s="48" t="n">
+      <c r="G121" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D121</f>
         <v>0</v>
       </c>
-      <c r="H121" s="48" t="n">
+      <c r="H121" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D121</f>
         <v>-0</v>
       </c>
-      <c r="I121" s="48" t="n">
+      <c r="I121" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D121</f>
         <v>0</v>
       </c>
-      <c r="J121" s="48" t="n">
+      <c r="J121" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D121</f>
         <v>0</v>
       </c>
-      <c r="K121" s="48" t="n">
+      <c r="K121" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D121</f>
         <v>0</v>
       </c>
-      <c r="L121" s="48" t="n">
+      <c r="L121" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D121</f>
         <v>0</v>
       </c>
@@ -7438,7 +7438,7 @@
         <f aca="false">+B74</f>
         <v>1104152</v>
       </c>
-      <c r="C122" s="59" t="inlineStr">
+      <c r="C122" s="58" t="inlineStr">
         <f aca="false">+D74</f>
         <is>
           <t/>
@@ -7448,31 +7448,31 @@
         <f aca="false">+I74</f>
         <v>0</v>
       </c>
-      <c r="E122" s="59" t="n">
+      <c r="E122" s="58" t="n">
         <f aca="false">+IF(D122&gt;0,C122+(SUMPRODUCT($G122:$L122,$G$141:$L$141)/$M122),0)</f>
         <v>0</v>
       </c>
-      <c r="G122" s="48" t="n">
+      <c r="G122" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D122</f>
         <v>0</v>
       </c>
-      <c r="H122" s="48" t="n">
+      <c r="H122" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D122</f>
         <v>-0</v>
       </c>
-      <c r="I122" s="48" t="n">
+      <c r="I122" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D122</f>
         <v>0</v>
       </c>
-      <c r="J122" s="48" t="n">
+      <c r="J122" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D122</f>
         <v>0</v>
       </c>
-      <c r="K122" s="48" t="n">
+      <c r="K122" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D122</f>
         <v>0</v>
       </c>
-      <c r="L122" s="48" t="n">
+      <c r="L122" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D122</f>
         <v>0</v>
       </c>
@@ -7486,7 +7486,7 @@
         <f aca="false">+B75</f>
         <v>1104136</v>
       </c>
-      <c r="C123" s="59" t="inlineStr">
+      <c r="C123" s="58" t="inlineStr">
         <f aca="false">+D75</f>
         <is>
           <t/>
@@ -7496,31 +7496,31 @@
         <f aca="false">+I75</f>
         <v>0</v>
       </c>
-      <c r="E123" s="59" t="n">
+      <c r="E123" s="58" t="n">
         <f aca="false">+IF(D123&gt;0,C123+(SUMPRODUCT($G123:$L123,$G$141:$L$141)/$M123),0)</f>
         <v>0</v>
       </c>
-      <c r="G123" s="48" t="n">
+      <c r="G123" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D123</f>
         <v>0</v>
       </c>
-      <c r="H123" s="48" t="n">
+      <c r="H123" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D123</f>
         <v>-0</v>
       </c>
-      <c r="I123" s="48" t="n">
+      <c r="I123" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D123</f>
         <v>0</v>
       </c>
-      <c r="J123" s="48" t="n">
+      <c r="J123" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D123</f>
         <v>0</v>
       </c>
-      <c r="K123" s="48" t="n">
+      <c r="K123" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D123</f>
         <v>0</v>
       </c>
-      <c r="L123" s="48" t="n">
+      <c r="L123" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D123</f>
         <v>0</v>
       </c>
@@ -7534,7 +7534,7 @@
         <f aca="false">+B76</f>
         <v>1104138</v>
       </c>
-      <c r="C124" s="59" t="inlineStr">
+      <c r="C124" s="58" t="inlineStr">
         <f aca="false">+D76</f>
         <is>
           <t/>
@@ -7544,31 +7544,31 @@
         <f aca="false">+I76</f>
         <v>0</v>
       </c>
-      <c r="E124" s="59" t="n">
+      <c r="E124" s="58" t="n">
         <f aca="false">+IF(D124&gt;0,C124+(SUMPRODUCT($G124:$L124,$G$141:$L$141)/$M124),0)</f>
         <v>0</v>
       </c>
-      <c r="G124" s="48" t="n">
+      <c r="G124" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D124</f>
         <v>0</v>
       </c>
-      <c r="H124" s="48" t="n">
+      <c r="H124" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D124</f>
         <v>-0</v>
       </c>
-      <c r="I124" s="48" t="n">
+      <c r="I124" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D124</f>
         <v>0</v>
       </c>
-      <c r="J124" s="48" t="n">
+      <c r="J124" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D124</f>
         <v>0</v>
       </c>
-      <c r="K124" s="48" t="n">
+      <c r="K124" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D124</f>
         <v>0</v>
       </c>
-      <c r="L124" s="48" t="n">
+      <c r="L124" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D124</f>
         <v>0</v>
       </c>
@@ -7582,7 +7582,7 @@
         <f aca="false">+B77</f>
         <v>1104139</v>
       </c>
-      <c r="C125" s="59" t="inlineStr">
+      <c r="C125" s="58" t="inlineStr">
         <f aca="false">+D77</f>
         <is>
           <t/>
@@ -7592,31 +7592,31 @@
         <f aca="false">+I77</f>
         <v>0</v>
       </c>
-      <c r="E125" s="59" t="n">
+      <c r="E125" s="58" t="n">
         <f aca="false">+IF(D125&gt;0,C125+(SUMPRODUCT($G125:$L125,$G$141:$L$141)/$M125),0)</f>
         <v>0</v>
       </c>
-      <c r="G125" s="48" t="n">
+      <c r="G125" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D125</f>
         <v>0</v>
       </c>
-      <c r="H125" s="48" t="n">
+      <c r="H125" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D125</f>
         <v>-0</v>
       </c>
-      <c r="I125" s="48" t="n">
+      <c r="I125" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D125</f>
         <v>0</v>
       </c>
-      <c r="J125" s="48" t="n">
+      <c r="J125" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D125</f>
         <v>0</v>
       </c>
-      <c r="K125" s="48" t="n">
+      <c r="K125" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D125</f>
         <v>0</v>
       </c>
-      <c r="L125" s="48" t="n">
+      <c r="L125" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D125</f>
         <v>0</v>
       </c>
@@ -7630,7 +7630,7 @@
         <f aca="false">+B78</f>
         <v>1104140</v>
       </c>
-      <c r="C126" s="59" t="inlineStr">
+      <c r="C126" s="58" t="inlineStr">
         <f aca="false">+D78</f>
         <is>
           <t/>
@@ -7640,31 +7640,31 @@
         <f aca="false">+I78</f>
         <v>0</v>
       </c>
-      <c r="E126" s="59" t="n">
+      <c r="E126" s="58" t="n">
         <f aca="false">+IF(D126&gt;0,C126+(SUMPRODUCT($G126:$L126,$G$141:$L$141)/$M126),0)</f>
         <v>0</v>
       </c>
-      <c r="G126" s="48" t="n">
+      <c r="G126" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D126</f>
         <v>0</v>
       </c>
-      <c r="H126" s="48" t="n">
+      <c r="H126" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D126</f>
         <v>-0</v>
       </c>
-      <c r="I126" s="48" t="n">
+      <c r="I126" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D126</f>
         <v>0</v>
       </c>
-      <c r="J126" s="48" t="n">
+      <c r="J126" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D126</f>
         <v>0</v>
       </c>
-      <c r="K126" s="48" t="n">
+      <c r="K126" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D126</f>
         <v>0</v>
       </c>
-      <c r="L126" s="48" t="n">
+      <c r="L126" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D126</f>
         <v>0</v>
       </c>
@@ -7678,7 +7678,7 @@
         <f aca="false">+B79</f>
         <v>1104141</v>
       </c>
-      <c r="C127" s="59" t="inlineStr">
+      <c r="C127" s="58" t="inlineStr">
         <f aca="false">+D79</f>
         <is>
           <t/>
@@ -7688,31 +7688,31 @@
         <f aca="false">+I79</f>
         <v>0</v>
       </c>
-      <c r="E127" s="59" t="n">
+      <c r="E127" s="58" t="n">
         <f aca="false">+IF(D127&gt;0,C127+(SUMPRODUCT($G127:$L127,$G$141:$L$141)/$M127),0)</f>
         <v>0</v>
       </c>
-      <c r="G127" s="48" t="n">
+      <c r="G127" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D127</f>
         <v>0</v>
       </c>
-      <c r="H127" s="48" t="n">
+      <c r="H127" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D127</f>
         <v>-0</v>
       </c>
-      <c r="I127" s="48" t="n">
+      <c r="I127" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D127</f>
         <v>0</v>
       </c>
-      <c r="J127" s="48" t="n">
+      <c r="J127" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D127</f>
         <v>0</v>
       </c>
-      <c r="K127" s="48" t="n">
+      <c r="K127" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D127</f>
         <v>0</v>
       </c>
-      <c r="L127" s="48" t="n">
+      <c r="L127" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D127</f>
         <v>0</v>
       </c>
@@ -7726,7 +7726,7 @@
         <f aca="false">+B80</f>
         <v>1104159</v>
       </c>
-      <c r="C128" s="59" t="inlineStr">
+      <c r="C128" s="58" t="inlineStr">
         <f aca="false">+D80</f>
         <is>
           <t/>
@@ -7736,31 +7736,31 @@
         <f aca="false">+I80</f>
         <v>0</v>
       </c>
-      <c r="E128" s="59" t="n">
+      <c r="E128" s="58" t="n">
         <f aca="false">+IF(D128&gt;0,C128+(SUMPRODUCT($G128:$L128,$G$141:$L$141)/$M128),0)</f>
         <v>0</v>
       </c>
-      <c r="G128" s="48" t="n">
+      <c r="G128" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D128</f>
         <v>0</v>
       </c>
-      <c r="H128" s="48" t="n">
+      <c r="H128" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D128</f>
         <v>-0</v>
       </c>
-      <c r="I128" s="48" t="n">
+      <c r="I128" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D128</f>
         <v>0</v>
       </c>
-      <c r="J128" s="48" t="n">
+      <c r="J128" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D128</f>
         <v>0</v>
       </c>
-      <c r="K128" s="48" t="n">
+      <c r="K128" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D128</f>
         <v>0</v>
       </c>
-      <c r="L128" s="48" t="n">
+      <c r="L128" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D128</f>
         <v>0</v>
       </c>
@@ -7774,7 +7774,7 @@
         <f aca="false">+B81</f>
         <v>1104161</v>
       </c>
-      <c r="C129" s="59" t="inlineStr">
+      <c r="C129" s="58" t="inlineStr">
         <f aca="false">+D81</f>
         <is>
           <t/>
@@ -7784,31 +7784,31 @@
         <f aca="false">+I81</f>
         <v>0</v>
       </c>
-      <c r="E129" s="59" t="n">
+      <c r="E129" s="58" t="n">
         <f aca="false">+IF(D129&gt;0,C129+(SUMPRODUCT($G129:$L129,$G$141:$L$141)/$M129),0)</f>
         <v>0</v>
       </c>
-      <c r="G129" s="48" t="n">
+      <c r="G129" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D129</f>
         <v>0</v>
       </c>
-      <c r="H129" s="48" t="n">
+      <c r="H129" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D129</f>
         <v>-0</v>
       </c>
-      <c r="I129" s="48" t="n">
+      <c r="I129" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D129</f>
         <v>0</v>
       </c>
-      <c r="J129" s="48" t="n">
+      <c r="J129" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D129</f>
         <v>0</v>
       </c>
-      <c r="K129" s="48" t="n">
+      <c r="K129" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D129</f>
         <v>0</v>
       </c>
-      <c r="L129" s="48" t="n">
+      <c r="L129" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D129</f>
         <v>0</v>
       </c>
@@ -7822,7 +7822,7 @@
         <f aca="false">+B82</f>
         <v>1104145</v>
       </c>
-      <c r="C130" s="59" t="inlineStr">
+      <c r="C130" s="58" t="inlineStr">
         <f aca="false">+D82</f>
         <is>
           <t/>
@@ -7832,31 +7832,31 @@
         <f aca="false">+I82</f>
         <v>0</v>
       </c>
-      <c r="E130" s="59" t="n">
+      <c r="E130" s="58" t="n">
         <f aca="false">+IF(D130&gt;0,C130+(SUMPRODUCT($G130:$L130,$G$141:$L$141)/$M130),0)</f>
         <v>0</v>
       </c>
-      <c r="G130" s="48" t="n">
+      <c r="G130" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D130</f>
         <v>0</v>
       </c>
-      <c r="H130" s="48" t="n">
+      <c r="H130" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D130</f>
         <v>-0</v>
       </c>
-      <c r="I130" s="48" t="n">
+      <c r="I130" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D130</f>
         <v>0</v>
       </c>
-      <c r="J130" s="48" t="n">
+      <c r="J130" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D130</f>
         <v>0</v>
       </c>
-      <c r="K130" s="48" t="n">
+      <c r="K130" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D130</f>
         <v>0</v>
       </c>
-      <c r="L130" s="48" t="n">
+      <c r="L130" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D130</f>
         <v>0</v>
       </c>
@@ -7870,7 +7870,7 @@
         <f aca="false">+B83</f>
         <v>1104133</v>
       </c>
-      <c r="C131" s="59" t="inlineStr">
+      <c r="C131" s="58" t="inlineStr">
         <f aca="false">+D83</f>
         <is>
           <t/>
@@ -7880,31 +7880,31 @@
         <f aca="false">+I83</f>
         <v>0</v>
       </c>
-      <c r="E131" s="59" t="n">
+      <c r="E131" s="58" t="n">
         <f aca="false">+IF(D131&gt;0,C131+(SUMPRODUCT($G131:$L131,$G$141:$L$141)/$M131),0)</f>
         <v>0</v>
       </c>
-      <c r="G131" s="48" t="n">
+      <c r="G131" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D131</f>
         <v>0</v>
       </c>
-      <c r="H131" s="48" t="n">
+      <c r="H131" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D131</f>
         <v>-0</v>
       </c>
-      <c r="I131" s="48" t="n">
+      <c r="I131" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D131</f>
         <v>0</v>
       </c>
-      <c r="J131" s="48" t="n">
+      <c r="J131" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D131</f>
         <v>0</v>
       </c>
-      <c r="K131" s="48" t="n">
+      <c r="K131" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D131</f>
         <v>0</v>
       </c>
-      <c r="L131" s="48" t="n">
+      <c r="L131" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D131</f>
         <v>0</v>
       </c>
@@ -7918,7 +7918,7 @@
         <f aca="false">+B84</f>
         <v>1104149</v>
       </c>
-      <c r="C132" s="59" t="inlineStr">
+      <c r="C132" s="58" t="inlineStr">
         <f aca="false">+D84</f>
         <is>
           <t/>
@@ -7928,31 +7928,31 @@
         <f aca="false">+I84</f>
         <v>0</v>
       </c>
-      <c r="E132" s="59" t="n">
+      <c r="E132" s="58" t="n">
         <f aca="false">+IF(D132&gt;0,C132+(SUMPRODUCT($G132:$L132,$G$141:$L$141)/$M132),0)</f>
         <v>0</v>
       </c>
-      <c r="G132" s="48" t="n">
+      <c r="G132" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D132</f>
         <v>0</v>
       </c>
-      <c r="H132" s="48" t="n">
+      <c r="H132" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D132</f>
         <v>-0</v>
       </c>
-      <c r="I132" s="48" t="n">
+      <c r="I132" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D132</f>
         <v>0</v>
       </c>
-      <c r="J132" s="48" t="n">
+      <c r="J132" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D132</f>
         <v>0</v>
       </c>
-      <c r="K132" s="48" t="n">
+      <c r="K132" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D132</f>
         <v>0</v>
       </c>
-      <c r="L132" s="48" t="n">
+      <c r="L132" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D132</f>
         <v>0</v>
       </c>
@@ -7966,7 +7966,7 @@
         <f aca="false">+B85</f>
         <v>1104151</v>
       </c>
-      <c r="C133" s="59" t="inlineStr">
+      <c r="C133" s="58" t="inlineStr">
         <f aca="false">+D85</f>
         <is>
           <t/>
@@ -7976,31 +7976,31 @@
         <f aca="false">+I85</f>
         <v>0</v>
       </c>
-      <c r="E133" s="59" t="n">
+      <c r="E133" s="58" t="n">
         <f aca="false">+IF(D133&gt;0,C133+(SUMPRODUCT($G133:$L133,$G$141:$L$141)/$M133),0)</f>
         <v>0</v>
       </c>
-      <c r="G133" s="48" t="n">
+      <c r="G133" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D133</f>
         <v>0</v>
       </c>
-      <c r="H133" s="48" t="n">
+      <c r="H133" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D133</f>
         <v>-0</v>
       </c>
-      <c r="I133" s="48" t="n">
+      <c r="I133" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D133</f>
         <v>0</v>
       </c>
-      <c r="J133" s="48" t="n">
+      <c r="J133" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D133</f>
         <v>0</v>
       </c>
-      <c r="K133" s="48" t="n">
+      <c r="K133" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D133</f>
         <v>0</v>
       </c>
-      <c r="L133" s="48" t="n">
+      <c r="L133" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D133</f>
         <v>0</v>
       </c>
@@ -8014,7 +8014,7 @@
         <f aca="false">+B86</f>
         <v>1104131</v>
       </c>
-      <c r="C134" s="59" t="inlineStr">
+      <c r="C134" s="58" t="inlineStr">
         <f aca="false">+D86</f>
         <is>
           <t/>
@@ -8024,31 +8024,31 @@
         <f aca="false">+I86</f>
         <v>0</v>
       </c>
-      <c r="E134" s="59" t="n">
+      <c r="E134" s="58" t="n">
         <f aca="false">+IF(D134&gt;0,C134+(SUMPRODUCT($G134:$L134,$G$141:$L$141)/$M134),0)</f>
         <v>0</v>
       </c>
-      <c r="G134" s="48" t="n">
+      <c r="G134" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D134</f>
         <v>0</v>
       </c>
-      <c r="H134" s="48" t="n">
+      <c r="H134" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D134</f>
         <v>-0</v>
       </c>
-      <c r="I134" s="48" t="n">
+      <c r="I134" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D134</f>
         <v>0</v>
       </c>
-      <c r="J134" s="48" t="n">
+      <c r="J134" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D134</f>
         <v>0</v>
       </c>
-      <c r="K134" s="48" t="n">
+      <c r="K134" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D134</f>
         <v>0</v>
       </c>
-      <c r="L134" s="48" t="n">
+      <c r="L134" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D134</f>
         <v>0</v>
       </c>
@@ -8062,7 +8062,7 @@
         <f aca="false">+B87</f>
         <v>1104155</v>
       </c>
-      <c r="C135" s="59" t="inlineStr">
+      <c r="C135" s="58" t="inlineStr">
         <f aca="false">+D87</f>
         <is>
           <t/>
@@ -8072,31 +8072,31 @@
         <f aca="false">+I87</f>
         <v>0</v>
       </c>
-      <c r="E135" s="59" t="n">
+      <c r="E135" s="58" t="n">
         <f aca="false">+IF(D135&gt;0,C135+(SUMPRODUCT($G135:$L135,$G$141:$L$141)/$M135),0)</f>
         <v>0</v>
       </c>
-      <c r="G135" s="48" t="n">
+      <c r="G135" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D135</f>
         <v>0</v>
       </c>
-      <c r="H135" s="48" t="n">
+      <c r="H135" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D135</f>
         <v>-0</v>
       </c>
-      <c r="I135" s="48" t="n">
+      <c r="I135" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D135</f>
         <v>0</v>
       </c>
-      <c r="J135" s="48" t="n">
+      <c r="J135" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D135</f>
         <v>0</v>
       </c>
-      <c r="K135" s="48" t="n">
+      <c r="K135" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D135</f>
         <v>0</v>
       </c>
-      <c r="L135" s="48" t="n">
+      <c r="L135" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D135</f>
         <v>0</v>
       </c>
@@ -8110,7 +8110,7 @@
         <f aca="false">+B88</f>
         <v>1104156</v>
       </c>
-      <c r="C136" s="59" t="inlineStr">
+      <c r="C136" s="58" t="inlineStr">
         <f aca="false">+D88</f>
         <is>
           <t/>
@@ -8120,31 +8120,31 @@
         <f aca="false">+I88</f>
         <v>0</v>
       </c>
-      <c r="E136" s="59" t="n">
+      <c r="E136" s="58" t="n">
         <f aca="false">+IF(D136&gt;0,C136+(SUMPRODUCT($G136:$L136,$G$141:$L$141)/$M136),0)</f>
         <v>0</v>
       </c>
-      <c r="G136" s="48" t="n">
+      <c r="G136" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D136</f>
         <v>0</v>
       </c>
-      <c r="H136" s="48" t="n">
+      <c r="H136" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D136</f>
         <v>-0</v>
       </c>
-      <c r="I136" s="48" t="n">
+      <c r="I136" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D136</f>
         <v>0</v>
       </c>
-      <c r="J136" s="48" t="n">
+      <c r="J136" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D136</f>
         <v>0</v>
       </c>
-      <c r="K136" s="48" t="n">
+      <c r="K136" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D136</f>
         <v>0</v>
       </c>
-      <c r="L136" s="48" t="n">
+      <c r="L136" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D136</f>
         <v>0</v>
       </c>
@@ -8158,7 +8158,7 @@
         <f aca="false">+B89</f>
         <v>1104157</v>
       </c>
-      <c r="C137" s="59" t="inlineStr">
+      <c r="C137" s="58" t="inlineStr">
         <f aca="false">+D89</f>
         <is>
           <t/>
@@ -8168,31 +8168,31 @@
         <f aca="false">+I89</f>
         <v>0</v>
       </c>
-      <c r="E137" s="59" t="n">
+      <c r="E137" s="58" t="n">
         <f aca="false">+IF(D137&gt;0,C137+(SUMPRODUCT($G137:$L137,$G$141:$L$141)/$M137),0)</f>
         <v>0</v>
       </c>
-      <c r="G137" s="48" t="n">
+      <c r="G137" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D137</f>
         <v>0</v>
       </c>
-      <c r="H137" s="48" t="n">
+      <c r="H137" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D137</f>
         <v>-0</v>
       </c>
-      <c r="I137" s="48" t="n">
+      <c r="I137" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D137</f>
         <v>0</v>
       </c>
-      <c r="J137" s="48" t="n">
+      <c r="J137" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D137</f>
         <v>0</v>
       </c>
-      <c r="K137" s="48" t="n">
+      <c r="K137" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D137</f>
         <v>0</v>
       </c>
-      <c r="L137" s="48" t="n">
+      <c r="L137" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D137</f>
         <v>0</v>
       </c>
@@ -8206,7 +8206,7 @@
         <f aca="false">+B90</f>
         <v>1104158</v>
       </c>
-      <c r="C138" s="59" t="inlineStr">
+      <c r="C138" s="58" t="inlineStr">
         <f aca="false">+D90</f>
         <is>
           <t/>
@@ -8216,31 +8216,31 @@
         <f aca="false">+I90</f>
         <v>0</v>
       </c>
-      <c r="E138" s="59" t="n">
+      <c r="E138" s="58" t="n">
         <f aca="false">+IF(D138&gt;0,C138+(SUMPRODUCT($G138:$L138,$G$141:$L$141)/$M138),0)</f>
         <v>0</v>
       </c>
-      <c r="G138" s="48" t="n">
+      <c r="G138" s="47" t="n">
         <f aca="false">+G$117/$M$117*$D138</f>
         <v>0</v>
       </c>
-      <c r="H138" s="48" t="n">
+      <c r="H138" s="47" t="n">
         <f aca="false">+H$117/$M$117*$D138</f>
         <v>-0</v>
       </c>
-      <c r="I138" s="48" t="n">
+      <c r="I138" s="47" t="n">
         <f aca="false">+I$117/$M$117*$D138</f>
         <v>0</v>
       </c>
-      <c r="J138" s="48" t="n">
+      <c r="J138" s="47" t="n">
         <f aca="false">+J$117/$M$117*$D138</f>
         <v>0</v>
       </c>
-      <c r="K138" s="48" t="n">
+      <c r="K138" s="47" t="n">
         <f aca="false">+K$117/$M$117*$D138</f>
         <v>0</v>
       </c>
-      <c r="L138" s="48" t="n">
+      <c r="L138" s="47" t="n">
         <f aca="false">+L$117/$M$117*$D138</f>
         <v>0</v>
       </c>
@@ -8254,7 +8254,7 @@
         <f aca="false">SUM(D119:D138)</f>
         <v>0</v>
       </c>
-      <c r="E139" s="59" t="e">
+      <c r="E139" s="58" t="e">
         <f aca="false">+SUMPRODUCT(D119:D138,E119:E138)/D139</f>
         <v>#DIV/0!</v>
       </c>
@@ -8288,7 +8288,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="140">
-      <c r="E140" s="60" t="inlineStr">
+      <c r="E140" s="59" t="inlineStr">
         <f aca="false">+E139-M148</f>
         <is>
           <t/>
@@ -8325,43 +8325,43 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="141">
       <c r="E141" s="18"/>
-      <c r="G141" s="61" t="inlineStr">
+      <c r="G141" s="60" t="inlineStr">
         <f aca="false">+G148-G140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H141" s="61" t="inlineStr">
+      <c r="H141" s="60" t="inlineStr">
         <f aca="false">+H148-H140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I141" s="61" t="inlineStr">
+      <c r="I141" s="60" t="inlineStr">
         <f aca="false">+I148-I140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J141" s="61" t="inlineStr">
+      <c r="J141" s="60" t="inlineStr">
         <f aca="false">+J148-J140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K141" s="61" t="inlineStr">
+      <c r="K141" s="60" t="inlineStr">
         <f aca="false">+K148-K140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="L141" s="61" t="inlineStr">
+      <c r="L141" s="60" t="inlineStr">
         <f aca="false">+L148-L140</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="M141" s="61" t="inlineStr">
+      <c r="M141" s="60" t="inlineStr">
         <f aca="false">+M148-M140</f>
         <is>
           <t/>
@@ -8372,7 +8372,7 @@
       <c r="B142" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D142" s="59" t="inlineStr">
+      <c r="D142" s="58" t="inlineStr">
         <f aca="false">+MAX(F8:F27,G36:L36)</f>
         <is>
           <t/>
@@ -8391,7 +8391,7 @@
       <c r="B143" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D143" s="62" t="inlineStr">
+      <c r="D143" s="61" t="inlineStr">
         <f aca="false">+M67</f>
         <is>
           <t/>
@@ -8410,7 +8410,7 @@
       <c r="B144" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D144" s="63" t="inlineStr">
+      <c r="D144" s="62" t="inlineStr">
         <f aca="false">+D142-D143</f>
         <is>
           <t/>
@@ -8429,14 +8429,14 @@
       <c r="B145" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="E145" s="64"/>
+      <c r="E145" s="63"/>
       <c r="G145" s="19" t="n">
         <f aca="false">+(1-G66)*$D$144</f>
         <v>0</v>
       </c>
       <c r="H145" s="19" t="n">
         <f aca="false">+(1-H66)*$D$144</f>
-        <v>-0.000700715648679136</v>
+        <v>-0.000462058033184417</v>
       </c>
       <c r="I145" s="19" t="n">
         <f aca="false">+(1-I66)*$D$144</f>
@@ -8444,15 +8444,15 @@
       </c>
       <c r="J145" s="19" t="n">
         <f aca="false">+(1-J66)*$D$144</f>
-        <v>0.00175178912169784</v>
+        <v>0.00115514508296104</v>
       </c>
       <c r="K145" s="19" t="n">
         <f aca="false">+(1-K66)*$D$144</f>
-        <v>0.00245250477037698</v>
+        <v>0.00161720311614546</v>
       </c>
       <c r="L145" s="19" t="n">
         <f aca="false">+(1-L66)*$D$144</f>
-        <v>0.00280286259471654</v>
+        <v>0.00184823213273767</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="146">
@@ -8535,37 +8535,37 @@
       </c>
       <c r="E148" s="25"/>
       <c r="F148" s="25"/>
-      <c r="G148" s="65" t="inlineStr">
+      <c r="G148" s="64" t="inlineStr">
         <f aca="false">+G146</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H148" s="65" t="inlineStr">
+      <c r="H148" s="64" t="inlineStr">
         <f aca="false">+H146</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I148" s="65" t="inlineStr">
+      <c r="I148" s="64" t="inlineStr">
         <f aca="false">+I146</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J148" s="65" t="inlineStr">
+      <c r="J148" s="64" t="inlineStr">
         <f aca="false">+J146</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K148" s="65" t="inlineStr">
+      <c r="K148" s="64" t="inlineStr">
         <f aca="false">+K146</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="L148" s="65" t="inlineStr">
+      <c r="L148" s="64" t="inlineStr">
         <f aca="false">+L146</f>
         <is>
           <t/>
@@ -8625,31 +8625,31 @@
       <c r="F152" s="40"/>
       <c r="G152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(G67),G146,((G139*G146)+(G65*G67))/G151)),0,+IF(ISERR(G67),G146,((G139*G146)+(G65*G67))/G151))</f>
-        <v>0.028625</v>
+        <v>0.024625</v>
       </c>
       <c r="H152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(H67),H146,((H139*H146)+(H65*H67))/H151)),0,+IF(ISERR(H67),H146,((H139*H146)+(H65*H67))/H151))</f>
-        <v>0.0297916666666667</v>
+        <v>0.0239583333333333</v>
       </c>
       <c r="I152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(I67),I146,((I139*I146)+(I65*I67))/I151)),0,+IF(ISERR(I67),I146,((I139*I146)+(I65*I67))/I151))</f>
-        <v>0.03125</v>
+        <v>0.0275</v>
       </c>
       <c r="J152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(J67),J146,((J139*J146)+(J65*J67))/J151)),0,+IF(ISERR(J67),J146,((J139*J146)+(J65*J67))/J151))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="K152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(K67),K146,((K139*K146)+(K65*K67))/K151)),0,+IF(ISERR(K67),K146,((K139*K146)+(K65*K67))/K151))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="L152" s="41" t="n">
         <f aca="false">+IF(ISERR(+IF(ISERR(L67),L146,((L139*L146)+(L65*L67))/L151)),0,+IF(ISERR(L67),L146,((L139*L146)+(L65*L67))/L151))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="M152" s="42" t="n">
         <f aca="false">+SUMPRODUCT(G151:L151,G152:L152)/M151</f>
-        <v>0.0314964217566043</v>
+        <v>0.0264397098340779</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="153">
@@ -8771,27 +8771,27 @@
         <f aca="false">+D159*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G159" s="48" t="n">
+      <c r="G159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*G$154),0,+$E159/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H159" s="48" t="n">
+      <c r="H159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*H$154),0,+$E159/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I159" s="48" t="n">
+      <c r="I159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*I$154),0,+$E159/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J159" s="48" t="n">
+      <c r="J159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*J$154),0,+$E159/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K159" s="48" t="n">
+      <c r="K159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*K$154),0,+$E159/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L159" s="48" t="n">
+      <c r="L159" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E159/$E$179*L$154),0,+$E159/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -8817,27 +8817,27 @@
         <f aca="false">+D160*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G160" s="48" t="n">
+      <c r="G160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*G$154),0,+$E160/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H160" s="48" t="n">
+      <c r="H160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*H$154),0,+$E160/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I160" s="48" t="n">
+      <c r="I160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*I$154),0,+$E160/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J160" s="48" t="n">
+      <c r="J160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*J$154),0,+$E160/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K160" s="48" t="n">
+      <c r="K160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*K$154),0,+$E160/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L160" s="48" t="n">
+      <c r="L160" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E160/$E$179*L$154),0,+$E160/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -8863,27 +8863,27 @@
         <f aca="false">+D161*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G161" s="48" t="n">
+      <c r="G161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*G$154),0,+$E161/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H161" s="48" t="n">
+      <c r="H161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*H$154),0,+$E161/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I161" s="48" t="n">
+      <c r="I161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*I$154),0,+$E161/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J161" s="48" t="n">
+      <c r="J161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*J$154),0,+$E161/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K161" s="48" t="n">
+      <c r="K161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*K$154),0,+$E161/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L161" s="48" t="n">
+      <c r="L161" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E161/$E$179*L$154),0,+$E161/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -8909,27 +8909,27 @@
         <f aca="false">+D162*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G162" s="48" t="n">
+      <c r="G162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*G$154),0,+$E162/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H162" s="48" t="n">
+      <c r="H162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*H$154),0,+$E162/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I162" s="48" t="n">
+      <c r="I162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*I$154),0,+$E162/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J162" s="48" t="n">
+      <c r="J162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*J$154),0,+$E162/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K162" s="48" t="n">
+      <c r="K162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*K$154),0,+$E162/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L162" s="48" t="n">
+      <c r="L162" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E162/$E$179*L$154),0,+$E162/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -8955,27 +8955,27 @@
         <f aca="false">+D163*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G163" s="48" t="n">
+      <c r="G163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*G$154),0,+$E163/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H163" s="48" t="n">
+      <c r="H163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*H$154),0,+$E163/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I163" s="48" t="n">
+      <c r="I163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*I$154),0,+$E163/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J163" s="48" t="n">
+      <c r="J163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*J$154),0,+$E163/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K163" s="48" t="n">
+      <c r="K163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*K$154),0,+$E163/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L163" s="48" t="n">
+      <c r="L163" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E163/$E$179*L$154),0,+$E163/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9001,27 +9001,27 @@
         <f aca="false">+D164*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G164" s="48" t="n">
+      <c r="G164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*G$154),0,+$E164/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H164" s="48" t="n">
+      <c r="H164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*H$154),0,+$E164/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I164" s="48" t="n">
+      <c r="I164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*I$154),0,+$E164/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J164" s="48" t="n">
+      <c r="J164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*J$154),0,+$E164/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K164" s="48" t="n">
+      <c r="K164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*K$154),0,+$E164/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L164" s="48" t="n">
+      <c r="L164" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E164/$E$179*L$154),0,+$E164/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9047,27 +9047,27 @@
         <f aca="false">+D165*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G165" s="48" t="n">
+      <c r="G165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*G$154),0,+$E165/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H165" s="48" t="n">
+      <c r="H165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*H$154),0,+$E165/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I165" s="48" t="n">
+      <c r="I165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*I$154),0,+$E165/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J165" s="48" t="n">
+      <c r="J165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*J$154),0,+$E165/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K165" s="48" t="n">
+      <c r="K165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*K$154),0,+$E165/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L165" s="48" t="n">
+      <c r="L165" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E165/$E$179*L$154),0,+$E165/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9093,27 +9093,27 @@
         <f aca="false">+D166*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G166" s="48" t="n">
+      <c r="G166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*G$154),0,+$E166/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H166" s="48" t="n">
+      <c r="H166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*H$154),0,+$E166/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I166" s="48" t="n">
+      <c r="I166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*I$154),0,+$E166/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J166" s="48" t="n">
+      <c r="J166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*J$154),0,+$E166/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K166" s="48" t="n">
+      <c r="K166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*K$154),0,+$E166/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L166" s="48" t="n">
+      <c r="L166" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E166/$E$179*L$154),0,+$E166/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9139,27 +9139,27 @@
         <f aca="false">+D167*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G167" s="48" t="n">
+      <c r="G167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*G$154),0,+$E167/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H167" s="48" t="n">
+      <c r="H167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*H$154),0,+$E167/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I167" s="48" t="n">
+      <c r="I167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*I$154),0,+$E167/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J167" s="48" t="n">
+      <c r="J167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*J$154),0,+$E167/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K167" s="48" t="n">
+      <c r="K167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*K$154),0,+$E167/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L167" s="48" t="n">
+      <c r="L167" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E167/$E$179*L$154),0,+$E167/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9185,27 +9185,27 @@
         <f aca="false">+D168*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G168" s="48" t="n">
+      <c r="G168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*G$154),0,+$E168/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H168" s="48" t="n">
+      <c r="H168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*H$154),0,+$E168/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I168" s="48" t="n">
+      <c r="I168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*I$154),0,+$E168/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J168" s="48" t="n">
+      <c r="J168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*J$154),0,+$E168/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K168" s="48" t="n">
+      <c r="K168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*K$154),0,+$E168/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L168" s="48" t="n">
+      <c r="L168" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E168/$E$179*L$154),0,+$E168/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9231,27 +9231,27 @@
         <f aca="false">+D169*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G169" s="48" t="n">
+      <c r="G169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*G$154),0,+$E169/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H169" s="48" t="n">
+      <c r="H169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*H$154),0,+$E169/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I169" s="48" t="n">
+      <c r="I169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*I$154),0,+$E169/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J169" s="48" t="n">
+      <c r="J169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*J$154),0,+$E169/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K169" s="48" t="n">
+      <c r="K169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*K$154),0,+$E169/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L169" s="48" t="n">
+      <c r="L169" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E169/$E$179*L$154),0,+$E169/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9277,27 +9277,27 @@
         <f aca="false">+D170*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G170" s="48" t="n">
+      <c r="G170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*G$154),0,+$E170/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H170" s="48" t="n">
+      <c r="H170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*H$154),0,+$E170/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I170" s="48" t="n">
+      <c r="I170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*I$154),0,+$E170/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J170" s="48" t="n">
+      <c r="J170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*J$154),0,+$E170/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K170" s="48" t="n">
+      <c r="K170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*K$154),0,+$E170/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L170" s="48" t="n">
+      <c r="L170" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E170/$E$179*L$154),0,+$E170/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9323,27 +9323,27 @@
         <f aca="false">+D171*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G171" s="48" t="n">
+      <c r="G171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*G$154),0,+$E171/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H171" s="48" t="n">
+      <c r="H171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*H$154),0,+$E171/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I171" s="48" t="n">
+      <c r="I171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*I$154),0,+$E171/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J171" s="48" t="n">
+      <c r="J171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*J$154),0,+$E171/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K171" s="48" t="n">
+      <c r="K171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*K$154),0,+$E171/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L171" s="48" t="n">
+      <c r="L171" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E171/$E$179*L$154),0,+$E171/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9369,27 +9369,27 @@
         <f aca="false">+D172*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G172" s="48" t="n">
+      <c r="G172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*G$154),0,+$E172/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H172" s="48" t="n">
+      <c r="H172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*H$154),0,+$E172/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I172" s="48" t="n">
+      <c r="I172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*I$154),0,+$E172/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J172" s="48" t="n">
+      <c r="J172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*J$154),0,+$E172/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K172" s="48" t="n">
+      <c r="K172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*K$154),0,+$E172/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L172" s="48" t="n">
+      <c r="L172" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E172/$E$179*L$154),0,+$E172/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9415,27 +9415,27 @@
         <f aca="false">+D173*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G173" s="48" t="n">
+      <c r="G173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*G$154),0,+$E173/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H173" s="48" t="n">
+      <c r="H173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*H$154),0,+$E173/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I173" s="48" t="n">
+      <c r="I173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*I$154),0,+$E173/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J173" s="48" t="n">
+      <c r="J173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*J$154),0,+$E173/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K173" s="48" t="n">
+      <c r="K173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*K$154),0,+$E173/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L173" s="48" t="n">
+      <c r="L173" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E173/$E$179*L$154),0,+$E173/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9461,27 +9461,27 @@
         <f aca="false">+D174*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G174" s="48" t="n">
+      <c r="G174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*G$154),0,+$E174/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H174" s="48" t="n">
+      <c r="H174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*H$154),0,+$E174/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I174" s="48" t="n">
+      <c r="I174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*I$154),0,+$E174/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J174" s="48" t="n">
+      <c r="J174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*J$154),0,+$E174/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K174" s="48" t="n">
+      <c r="K174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*K$154),0,+$E174/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L174" s="48" t="n">
+      <c r="L174" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E174/$E$179*L$154),0,+$E174/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9507,27 +9507,27 @@
         <f aca="false">+D175*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G175" s="48" t="n">
+      <c r="G175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*G$154),0,+$E175/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H175" s="48" t="n">
+      <c r="H175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*H$154),0,+$E175/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I175" s="48" t="n">
+      <c r="I175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*I$154),0,+$E175/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J175" s="48" t="n">
+      <c r="J175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*J$154),0,+$E175/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K175" s="48" t="n">
+      <c r="K175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*K$154),0,+$E175/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L175" s="48" t="n">
+      <c r="L175" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E175/$E$179*L$154),0,+$E175/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9553,27 +9553,27 @@
         <f aca="false">+D176*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G176" s="48" t="n">
+      <c r="G176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*G$154),0,+$E176/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H176" s="48" t="n">
+      <c r="H176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*H$154),0,+$E176/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I176" s="48" t="n">
+      <c r="I176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*I$154),0,+$E176/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J176" s="48" t="n">
+      <c r="J176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*J$154),0,+$E176/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K176" s="48" t="n">
+      <c r="K176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*K$154),0,+$E176/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L176" s="48" t="n">
+      <c r="L176" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E176/$E$179*L$154),0,+$E176/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9599,27 +9599,27 @@
         <f aca="false">+D177*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G177" s="48" t="n">
+      <c r="G177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*G$154),0,+$E177/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H177" s="48" t="n">
+      <c r="H177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*H$154),0,+$E177/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I177" s="48" t="n">
+      <c r="I177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*I$154),0,+$E177/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J177" s="48" t="n">
+      <c r="J177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*J$154),0,+$E177/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K177" s="48" t="n">
+      <c r="K177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*K$154),0,+$E177/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L177" s="48" t="n">
+      <c r="L177" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E177/$E$179*L$154),0,+$E177/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9645,27 +9645,27 @@
         <f aca="false">+D178*$D$181</f>
         <v>0</v>
       </c>
-      <c r="G178" s="48" t="n">
+      <c r="G178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*G$154),0,+$E178/$E$179*G$154)</f>
         <v>0</v>
       </c>
-      <c r="H178" s="48" t="n">
+      <c r="H178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*H$154),0,+$E178/$E$179*H$154)</f>
         <v>0</v>
       </c>
-      <c r="I178" s="48" t="n">
+      <c r="I178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*I$154),0,+$E178/$E$179*I$154)</f>
         <v>0</v>
       </c>
-      <c r="J178" s="48" t="n">
+      <c r="J178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*J$154),0,+$E178/$E$179*J$154)</f>
         <v>0</v>
       </c>
-      <c r="K178" s="48" t="n">
+      <c r="K178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*K$154),0,+$E178/$E$179*K$154)</f>
         <v>0</v>
       </c>
-      <c r="L178" s="48" t="n">
+      <c r="L178" s="47" t="n">
         <f aca="false">+IF(ISERR(+$E178/$E$179*L$154),0,+$E178/$E$179*L$154)</f>
         <v>0</v>
       </c>
@@ -9711,7 +9711,7 @@
       <c r="B181" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D181" s="66" t="n">
+      <c r="D181" s="65" t="n">
         <f aca="false">+IF(ISERR(D180/D179),0,D180/D179)</f>
         <v>0</v>
       </c>
@@ -9719,12 +9719,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="14" outlineLevel="1" r="182">
       <c r="E182" s="18"/>
-      <c r="H182" s="59"/>
-      <c r="I182" s="59"/>
-      <c r="J182" s="59"/>
-      <c r="K182" s="59"/>
-      <c r="L182" s="59"/>
-      <c r="M182" s="59"/>
+      <c r="H182" s="58"/>
+      <c r="I182" s="58"/>
+      <c r="J182" s="58"/>
+      <c r="K182" s="58"/>
+      <c r="L182" s="58"/>
+      <c r="M182" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="183">
       <c r="D183" s="20" t="s">
@@ -9767,37 +9767,37 @@
       </c>
       <c r="E184" s="25"/>
       <c r="F184" s="25"/>
-      <c r="G184" s="65" t="inlineStr">
+      <c r="G184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(G67),G146,MAX(G67,G146))</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H184" s="65" t="inlineStr">
+      <c r="H184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(H67),H146,MAX(H67,H146))</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="I184" s="65" t="inlineStr">
+      <c r="I184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(I67),I146,MAX(I67,I146))</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J184" s="65" t="inlineStr">
+      <c r="J184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(J67),J146,MAX(J67,J146))</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K184" s="65" t="inlineStr">
+      <c r="K184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(K67),K146,MAX(K67,K146))</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="L184" s="65" t="inlineStr">
+      <c r="L184" s="64" t="inlineStr">
         <f aca="false">+IF(ISERROR(L67),L146,MAX(L67,L146))</f>
         <is>
           <t/>
@@ -9856,31 +9856,31 @@
       <c r="F187" s="40"/>
       <c r="G187" s="41" t="n">
         <f aca="false">+IF(G186=0,0,IF(ISERR(G152),G184,((G183*G184)+(G151*G152))/G186))</f>
-        <v>0.028625</v>
+        <v>0.024625</v>
       </c>
       <c r="H187" s="41" t="n">
         <f aca="false">+IF(H186=0,0,IF(ISERR(H152),H184,((H183*H184)+(H151*H152))/H186))</f>
-        <v>0.0297916666666667</v>
+        <v>0.0239583333333333</v>
       </c>
       <c r="I187" s="41" t="n">
         <f aca="false">+IF(I186=0,0,IF(ISERR(I152),I184,((I183*I184)+(I151*I152))/I186))</f>
-        <v>0.03125</v>
+        <v>0.0275</v>
       </c>
       <c r="J187" s="41" t="n">
         <f aca="false">+IF(J186=0,0,IF(ISERR(J152),J184,((J183*J184)+(J151*J152))/J186))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="K187" s="41" t="n">
         <f aca="false">+IF(K186=0,0,IF(ISERR(K152),K184,((K183*K184)+(K151*K152))/K186))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="L187" s="41" t="n">
         <f aca="false">+IF(L186=0,0,IF(ISERR(L152),L184,((L183*L184)+(L151*L152))/L186))</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="M187" s="42" t="n">
         <f aca="false">+SUMPRODUCT(G187:L187*G186:L186)/M186</f>
-        <v>0.0314964217566043</v>
+        <v>0.0264397098340779</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="188">
@@ -9981,9 +9981,9 @@
         <f aca="false">+'bid input'!B2</f>
         <v>1104134</v>
       </c>
-      <c r="C195" s="59" t="n">
+      <c r="C195" s="58" t="n">
         <f aca="false">+IF(D195&gt;0,IF(M8&gt;0,F8,0)+IF(M37&gt;0,SUMPRODUCT(G$36:L$36,G37:L37)/M37,0)+E119+IF(M159&gt;0,M$184,0),0)</f>
-        <v>0.035</v>
+        <v>0.025</v>
       </c>
       <c r="D195" s="14" t="n">
         <f aca="false">+M195</f>
@@ -10024,7 +10024,7 @@
         <f aca="false">+'bid input'!B3</f>
         <v>1104143</v>
       </c>
-      <c r="C196" s="59" t="n">
+      <c r="C196" s="58" t="n">
         <f aca="false">+IF(D196&gt;0,IF(M9&gt;0,F9,0)+IF(M38&gt;0,SUMPRODUCT(G$36:L$36,G38:L38)/M38,0)+E120+IF(M160&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10067,7 +10067,7 @@
         <f aca="false">+'bid input'!B4</f>
         <v>1104154</v>
       </c>
-      <c r="C197" s="59" t="n">
+      <c r="C197" s="58" t="n">
         <f aca="false">+IF(D197&gt;0,IF(M10&gt;0,F10,0)+IF(M39&gt;0,SUMPRODUCT(G$36:L$36,G39:L39)/M39,0)+E121+IF(M161&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10110,7 +10110,7 @@
         <f aca="false">+'bid input'!B5</f>
         <v>1104152</v>
       </c>
-      <c r="C198" s="59" t="n">
+      <c r="C198" s="58" t="n">
         <f aca="false">+IF(D198&gt;0,IF(M11&gt;0,F11,0)+IF(M40&gt;0,SUMPRODUCT(G$36:L$36,G40:L40)/M40,0)+E122+IF(M162&gt;0,M$184,0),0)</f>
         <v>0.025</v>
       </c>
@@ -10153,7 +10153,7 @@
         <f aca="false">+'bid input'!B6</f>
         <v>1104136</v>
       </c>
-      <c r="C199" s="59" t="n">
+      <c r="C199" s="58" t="n">
         <f aca="false">+IF(D199&gt;0,IF(M12&gt;0,F12,0)+IF(M41&gt;0,SUMPRODUCT(G$36:L$36,G41:L41)/M41,0)+E123+IF(M163&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10196,7 +10196,7 @@
         <f aca="false">+'bid input'!B7</f>
         <v>1104138</v>
       </c>
-      <c r="C200" s="59" t="n">
+      <c r="C200" s="58" t="n">
         <f aca="false">+IF(D200&gt;0,IF(M13&gt;0,F13,0)+IF(M42&gt;0,SUMPRODUCT(G$36:L$36,G42:L42)/M42,0)+E124+IF(M164&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10239,7 +10239,7 @@
         <f aca="false">+'bid input'!B8</f>
         <v>1104139</v>
       </c>
-      <c r="C201" s="59" t="n">
+      <c r="C201" s="58" t="n">
         <f aca="false">+IF(D201&gt;0,IF(M14&gt;0,F14,0)+IF(M43&gt;0,SUMPRODUCT(G$36:L$36,G43:L43)/M43,0)+E125+IF(M165&gt;0,M$184,0),0)</f>
         <v>0.0225</v>
       </c>
@@ -10282,7 +10282,7 @@
         <f aca="false">+'bid input'!B9</f>
         <v>1104140</v>
       </c>
-      <c r="C202" s="59" t="n">
+      <c r="C202" s="58" t="n">
         <f aca="false">+IF(D202&gt;0,IF(M15&gt;0,F15,0)+IF(M44&gt;0,SUMPRODUCT(G$36:L$36,G44:L44)/M44,0)+E126+IF(M166&gt;0,M$184,0),0)</f>
         <v>0.02875</v>
       </c>
@@ -10325,9 +10325,9 @@
         <f aca="false">+'bid input'!B10</f>
         <v>1104141</v>
       </c>
-      <c r="C203" s="59" t="n">
+      <c r="C203" s="58" t="n">
         <f aca="false">+IF(D203&gt;0,IF(M16&gt;0,F16,0)+IF(M45&gt;0,SUMPRODUCT(G$36:L$36,G45:L45)/M45,0)+E127+IF(M167&gt;0,M$184,0),0)</f>
-        <v>0.035</v>
+        <v>0.025</v>
       </c>
       <c r="D203" s="14" t="n">
         <f aca="false">+M203</f>
@@ -10367,7 +10367,7 @@
         <f aca="false">+'bid input'!B11</f>
         <v>1104159</v>
       </c>
-      <c r="C204" s="59" t="n">
+      <c r="C204" s="58" t="n">
         <f aca="false">+IF(D204&gt;0,IF(M17&gt;0,F17,0)+IF(M46&gt;0,SUMPRODUCT(G$36:L$36,G46:L46)/M46,0)+E128+IF(M168&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10409,7 +10409,7 @@
         <f aca="false">+'bid input'!B12</f>
         <v>1104161</v>
       </c>
-      <c r="C205" s="59" t="n">
+      <c r="C205" s="58" t="n">
         <f aca="false">+IF(D205&gt;0,IF(M18&gt;0,F18,0)+IF(M47&gt;0,SUMPRODUCT(G$36:L$36,G47:L47)/M47,0)+E129+IF(M169&gt;0,M$184,0),0)</f>
         <v>0.025</v>
       </c>
@@ -10451,7 +10451,7 @@
         <f aca="false">+'bid input'!B13</f>
         <v>1104145</v>
       </c>
-      <c r="C206" s="59" t="n">
+      <c r="C206" s="58" t="n">
         <f aca="false">+IF(D206&gt;0,IF(M19&gt;0,F19,0)+IF(M48&gt;0,SUMPRODUCT(G$36:L$36,G48:L48)/M48,0)+E130+IF(M170&gt;0,M$184,0),0)</f>
         <v>0.02375</v>
       </c>
@@ -10493,9 +10493,9 @@
         <f aca="false">+'bid input'!B14</f>
         <v>1104133</v>
       </c>
-      <c r="C207" s="59" t="n">
+      <c r="C207" s="58" t="n">
         <f aca="false">+IF(D207&gt;0,IF(M20&gt;0,F20,0)+IF(M49&gt;0,SUMPRODUCT(G$36:L$36,G49:L49)/M49,0)+E131+IF(M171&gt;0,M$184,0),0)</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="D207" s="14" t="n">
         <f aca="false">+M207</f>
@@ -10535,9 +10535,9 @@
         <f aca="false">+'bid input'!B15</f>
         <v>1104149</v>
       </c>
-      <c r="C208" s="59" t="n">
+      <c r="C208" s="58" t="n">
         <f aca="false">+IF(D208&gt;0,IF(M21&gt;0,F21,0)+IF(M50&gt;0,SUMPRODUCT(G$36:L$36,G50:L50)/M50,0)+E132+IF(M172&gt;0,M$184,0),0)</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="D208" s="14" t="n">
         <f aca="false">+M208</f>
@@ -10577,7 +10577,7 @@
         <f aca="false">+'bid input'!B16</f>
         <v>1104151</v>
       </c>
-      <c r="C209" s="59" t="n">
+      <c r="C209" s="58" t="n">
         <f aca="false">+IF(D209&gt;0,IF(M22&gt;0,F22,0)+IF(M51&gt;0,SUMPRODUCT(G$36:L$36,G51:L51)/M51,0)+E133+IF(M173&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10619,7 +10619,7 @@
         <f aca="false">+'bid input'!B17</f>
         <v>1104131</v>
       </c>
-      <c r="C210" s="59" t="n">
+      <c r="C210" s="58" t="n">
         <f aca="false">+IF(D210&gt;0,IF(M23&gt;0,F23,0)+IF(M52&gt;0,SUMPRODUCT(G$36:L$36,G52:L52)/M52,0)+E134+IF(M174&gt;0,M$184,0),0)</f>
         <v>0.025</v>
       </c>
@@ -10661,7 +10661,7 @@
         <f aca="false">+'bid input'!B18</f>
         <v>1104155</v>
       </c>
-      <c r="C211" s="59" t="n">
+      <c r="C211" s="58" t="n">
         <f aca="false">+IF(D211&gt;0,IF(M24&gt;0,F24,0)+IF(M53&gt;0,SUMPRODUCT(G$36:L$36,G53:L53)/M53,0)+E135+IF(M175&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10703,9 +10703,9 @@
         <f aca="false">+'bid input'!B19</f>
         <v>1104156</v>
       </c>
-      <c r="C212" s="59" t="n">
+      <c r="C212" s="58" t="n">
         <f aca="false">+IF(D212&gt;0,IF(M25&gt;0,F25,0)+IF(M54&gt;0,SUMPRODUCT(G$36:L$36,G54:L54)/M54,0)+E136+IF(M176&gt;0,M$184,0),0)</f>
-        <v>0.035</v>
+        <v>0.02875</v>
       </c>
       <c r="D212" s="14" t="n">
         <f aca="false">+M212</f>
@@ -10745,7 +10745,7 @@
         <f aca="false">+'bid input'!B20</f>
         <v>1104157</v>
       </c>
-      <c r="C213" s="59" t="n">
+      <c r="C213" s="58" t="n">
         <f aca="false">+IF(D213&gt;0,IF(M26&gt;0,F26,0)+IF(M55&gt;0,SUMPRODUCT(G$36:L$36,G55:L55)/M55,0)+E137+IF(M177&gt;0,M$184,0),0)</f>
         <v>0.02</v>
       </c>
@@ -10787,7 +10787,7 @@
         <f aca="false">+'bid input'!B21</f>
         <v>1104158</v>
       </c>
-      <c r="C214" s="59" t="n">
+      <c r="C214" s="58" t="n">
         <f aca="false">+IF(D214&gt;0,IF(M27&gt;0,F27,0)+IF(M56&gt;0,SUMPRODUCT(G$36:L$36,G56:L56)/M56,0)+E138+IF(M178&gt;0,M$184,0),0)</f>
         <v>0</v>
       </c>
@@ -10828,9 +10828,9 @@
       <c r="B215" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C215" s="59" t="n">
+      <c r="C215" s="58" t="n">
         <f aca="false">+SUMPRODUCT(C195:C214,M195:M214)/M215</f>
-        <v>0.0302023502066116</v>
+        <v>0.0263525740358127</v>
       </c>
       <c r="D215" s="14" t="n">
         <f aca="false">SUM(D195:D214)</f>
@@ -10866,7 +10866,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="216">
-      <c r="C216" s="59"/>
+      <c r="C216" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="217">
       <c r="B217" s="0" t="s">
@@ -10886,61 +10886,61 @@
           <t/>
         </is>
       </c>
-      <c r="G219" s="59" t="inlineStr">
+      <c r="G219" s="58" t="inlineStr">
         <f aca="false">+IF(G190="NA",G187+$C$217,0)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="H219" s="59" t="n">
+      <c r="H219" s="58" t="n">
         <f aca="false">+IF(H190="NA",H187+$C$217,0)</f>
         <v>0</v>
       </c>
-      <c r="I219" s="59" t="inlineStr">
+      <c r="I219" s="58" t="inlineStr">
         <f aca="false">+IF(I190="NA",I187+$C$217,0)</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J219" s="59" t="n">
+      <c r="J219" s="58" t="n">
         <f aca="false">+IF(J190="NA",J187+$C$217,0)</f>
         <v>0</v>
       </c>
-      <c r="K219" s="59" t="n">
+      <c r="K219" s="58" t="n">
         <f aca="false">+IF(K190="NA",K187+$C$217,0)</f>
         <v>0</v>
       </c>
-      <c r="L219" s="59" t="n">
+      <c r="L219" s="58" t="n">
         <f aca="false">+IF(L190="NA",L187+$C$217,0)</f>
         <v>0</v>
       </c>
-      <c r="M219" s="59" t="n">
+      <c r="M219" s="58" t="n">
         <f aca="false">+SUMPRODUCT(G215:L215,G219:L219)/M215</f>
-        <v>0.0402023502066116</v>
+        <v>0.0363525740358127</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
-      <c r="G220" s="67" t="str">
+      <c r="G220" s="66" t="str">
         <f aca="false">+IF(G219=0, "NOT FUNDED","")</f>
         <v/>
       </c>
-      <c r="H220" s="67" t="str">
+      <c r="H220" s="66" t="str">
         <f aca="false">+IF(H219=0, "NOT FUNDED","")</f>
         <v>NOT FUNDED</v>
       </c>
-      <c r="I220" s="67" t="str">
+      <c r="I220" s="66" t="str">
         <f aca="false">+IF(I219=0, "NOT FUNDED","")</f>
         <v/>
       </c>
-      <c r="J220" s="67" t="str">
+      <c r="J220" s="66" t="str">
         <f aca="false">+IF(J219=0, "NOT FUNDED","")</f>
         <v>NOT FUNDED</v>
       </c>
-      <c r="K220" s="67" t="str">
+      <c r="K220" s="66" t="str">
         <f aca="false">+IF(K219=0, "NOT FUNDED","")</f>
         <v>NOT FUNDED</v>
       </c>
-      <c r="L220" s="67" t="str">
+      <c r="L220" s="66" t="str">
         <f aca="false">+IF(L219=0, "NOT FUNDED","")</f>
         <v>NOT FUNDED</v>
       </c>

</xml_diff>